<commit_message>
contact us form, format amount for locale and bug fixes
</commit_message>
<xml_diff>
--- a/spreadsheets/BudgetManager.xlsx
+++ b/spreadsheets/BudgetManager.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D900"/>
+  <dimension ref="A1:D978"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6628,7 +6628,7 @@
         <v>574</v>
       </c>
       <c r="D451" t="str">
-        <v>Bank Credit</v>
+        <v>Bank Credit Interest</v>
       </c>
     </row>
     <row r="452">
@@ -10039,72 +10039,72 @@
     </row>
     <row r="697">
       <c r="A697" t="str">
-        <v>2021-10-03</v>
+        <v>2021-09-14</v>
       </c>
       <c r="B697" t="str">
-        <v>Other Income</v>
+        <v>Food</v>
       </c>
       <c r="C697">
-        <v>1892</v>
+        <v>787</v>
       </c>
       <c r="D697" t="str">
-        <v>Bank Interest</v>
+        <v>Big basket</v>
       </c>
     </row>
     <row r="698">
       <c r="A698" t="str">
-        <v>2021-09-14</v>
+        <v>2021-10-25</v>
       </c>
       <c r="B698" t="str">
         <v>Food</v>
       </c>
       <c r="C698">
-        <v>787</v>
+        <v>168</v>
       </c>
       <c r="D698" t="str">
-        <v>Big basket</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="699">
       <c r="A699" t="str">
-        <v>2021-10-25</v>
+        <v>2021-10-17</v>
       </c>
       <c r="B699" t="str">
-        <v>Food</v>
+        <v>Home</v>
       </c>
       <c r="C699">
-        <v>168</v>
+        <v>60</v>
       </c>
       <c r="D699" t="str">
-        <v>Swiggy</v>
+        <v>Garbage</v>
       </c>
     </row>
     <row r="700">
       <c r="A700" t="str">
-        <v>2021-10-17</v>
+        <v>2021-10-23</v>
       </c>
       <c r="B700" t="str">
-        <v>Home</v>
+        <v>Food</v>
       </c>
       <c r="C700">
-        <v>60</v>
+        <v>168</v>
       </c>
       <c r="D700" t="str">
-        <v>Garbage</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="701">
       <c r="A701" t="str">
-        <v>2021-10-23</v>
+        <v>2021-11-27</v>
       </c>
       <c r="B701" t="str">
-        <v>Food</v>
+        <v>Bills</v>
       </c>
       <c r="C701">
-        <v>168</v>
+        <v>589</v>
       </c>
       <c r="D701" t="str">
-        <v>Swiggy</v>
+        <v>Airtel Wifi Delhi</v>
       </c>
     </row>
     <row r="702">
@@ -10115,24 +10115,24 @@
         <v>Bills</v>
       </c>
       <c r="C702">
-        <v>589</v>
+        <v>1299</v>
       </c>
       <c r="D702" t="str">
-        <v>Airtel Wifi Delhi</v>
+        <v>Jio Recharge</v>
       </c>
     </row>
     <row r="703">
       <c r="A703" t="str">
-        <v>2021-11-27</v>
+        <v>2021-10-30</v>
       </c>
       <c r="B703" t="str">
-        <v>Bills</v>
+        <v>Other Income</v>
       </c>
       <c r="C703">
-        <v>1299</v>
+        <v>690</v>
       </c>
       <c r="D703" t="str">
-        <v>Jio Recharge</v>
+        <v>Amazon Pay Cashback</v>
       </c>
     </row>
     <row r="704">
@@ -10140,24 +10140,24 @@
         <v>2021-10-30</v>
       </c>
       <c r="B704" t="str">
-        <v>Other Income</v>
+        <v>Food</v>
       </c>
       <c r="C704">
-        <v>690</v>
+        <v>100</v>
       </c>
       <c r="D704" t="str">
-        <v>Amazon Pay Cashback</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="705">
       <c r="A705" t="str">
-        <v>2021-10-30</v>
+        <v>2021-10-16</v>
       </c>
       <c r="B705" t="str">
         <v>Food</v>
       </c>
       <c r="C705">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D705" t="str">
         <v>Swiggy</v>
@@ -10165,30 +10165,30 @@
     </row>
     <row r="706">
       <c r="A706" t="str">
-        <v>2021-10-16</v>
+        <v>2021-10-17</v>
       </c>
       <c r="B706" t="str">
-        <v>Food</v>
+        <v>Home</v>
       </c>
       <c r="C706">
-        <v>150</v>
+        <v>9000</v>
       </c>
       <c r="D706" t="str">
-        <v>Swiggy</v>
+        <v>Rent</v>
       </c>
     </row>
     <row r="707">
       <c r="A707" t="str">
-        <v>2021-10-17</v>
+        <v>2021-12-05</v>
       </c>
       <c r="B707" t="str">
         <v>Home</v>
       </c>
       <c r="C707">
-        <v>9000</v>
+        <v>900</v>
       </c>
       <c r="D707" t="str">
-        <v>Rent</v>
+        <v>LPG</v>
       </c>
     </row>
     <row r="708">
@@ -10196,279 +10196,279 @@
         <v>2021-12-05</v>
       </c>
       <c r="B708" t="str">
-        <v>Home</v>
+        <v>Other Income</v>
       </c>
       <c r="C708">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="D708" t="str">
-        <v>LPG</v>
+        <v>From Papa</v>
       </c>
     </row>
     <row r="709">
       <c r="A709" t="str">
-        <v>2021-12-05</v>
+        <v>2021-11-27</v>
       </c>
       <c r="B709" t="str">
-        <v>Other Income</v>
+        <v>Shopping</v>
       </c>
       <c r="C709">
-        <v>500</v>
+        <v>1100</v>
       </c>
       <c r="D709" t="str">
-        <v>From Papa</v>
+        <v>Specs</v>
       </c>
     </row>
     <row r="710">
       <c r="A710" t="str">
-        <v>2021-11-27</v>
+        <v>2021-12-21</v>
       </c>
       <c r="B710" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C710">
-        <v>1100</v>
+        <v>125</v>
       </c>
       <c r="D710" t="str">
-        <v>Specs</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="711">
       <c r="A711" t="str">
-        <v>2021-12-21</v>
+        <v>2021-12-22</v>
       </c>
       <c r="B711" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C711">
-        <v>125</v>
+        <v>713</v>
       </c>
       <c r="D711" t="str">
-        <v>Swiggy</v>
+        <v>Amazon</v>
       </c>
     </row>
     <row r="712">
       <c r="A712" t="str">
-        <v>2021-12-22</v>
+        <v>2021-12-06</v>
       </c>
       <c r="B712" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C712">
-        <v>713</v>
+        <v>97</v>
       </c>
       <c r="D712" t="str">
-        <v>Amazon</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="713">
       <c r="A713" t="str">
-        <v>2021-12-06</v>
+        <v>2021-12-20</v>
       </c>
       <c r="B713" t="str">
         <v>Food</v>
       </c>
       <c r="C713">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D713" t="str">
-        <v>Swiggy</v>
+        <v>Water And Dairy</v>
       </c>
     </row>
     <row r="714">
       <c r="A714" t="str">
-        <v>2021-12-20</v>
+        <v>2021-10-18</v>
       </c>
       <c r="B714" t="str">
         <v>Food</v>
       </c>
       <c r="C714">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="D714" t="str">
-        <v>Water And Dairy</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="715">
       <c r="A715" t="str">
-        <v>2021-10-18</v>
+        <v>2021-10-28</v>
       </c>
       <c r="B715" t="str">
-        <v>Food</v>
+        <v>Bills</v>
       </c>
       <c r="C715">
-        <v>137</v>
+        <v>588</v>
       </c>
       <c r="D715" t="str">
-        <v>Swiggy</v>
+        <v>Airtel Wifi</v>
       </c>
     </row>
     <row r="716">
       <c r="A716" t="str">
-        <v>2021-10-28</v>
+        <v>2021-11-01</v>
       </c>
       <c r="B716" t="str">
-        <v>Bills</v>
+        <v>Other Income</v>
       </c>
       <c r="C716">
-        <v>588</v>
+        <v>2100</v>
       </c>
       <c r="D716" t="str">
-        <v>Airtel Wifi</v>
+        <v>Diwali Bonus</v>
       </c>
     </row>
     <row r="717">
       <c r="A717" t="str">
-        <v>2021-11-01</v>
+        <v>2021-12-17</v>
       </c>
       <c r="B717" t="str">
-        <v>Other Income</v>
+        <v>Food</v>
       </c>
       <c r="C717">
-        <v>2100</v>
+        <v>163</v>
       </c>
       <c r="D717" t="str">
-        <v>Diwali Bonus</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="718">
       <c r="A718" t="str">
-        <v>2021-12-17</v>
+        <v>2021-11-27</v>
       </c>
       <c r="B718" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C718">
-        <v>163</v>
+        <v>319</v>
       </c>
       <c r="D718" t="str">
-        <v>Swiggy</v>
+        <v>Amazon</v>
       </c>
     </row>
     <row r="719">
       <c r="A719" t="str">
-        <v>2021-11-27</v>
+        <v>2021-12-11</v>
       </c>
       <c r="B719" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C719">
-        <v>319</v>
+        <v>130</v>
       </c>
       <c r="D719" t="str">
-        <v>Amazon</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="720">
       <c r="A720" t="str">
-        <v>2021-12-11</v>
+        <v>2021-12-17</v>
       </c>
       <c r="B720" t="str">
         <v>Food</v>
       </c>
       <c r="C720">
-        <v>130</v>
+        <v>1090</v>
       </c>
       <c r="D720" t="str">
-        <v>Swiggy</v>
+        <v>Bigbasket</v>
       </c>
     </row>
     <row r="721">
       <c r="A721" t="str">
-        <v>2021-12-17</v>
+        <v>2021-10-21</v>
       </c>
       <c r="B721" t="str">
         <v>Food</v>
       </c>
       <c r="C721">
-        <v>1090</v>
+        <v>140</v>
       </c>
       <c r="D721" t="str">
-        <v>Bigbasket</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="722">
       <c r="A722" t="str">
-        <v>2021-10-21</v>
+        <v>2021-12-15</v>
       </c>
       <c r="B722" t="str">
         <v>Food</v>
       </c>
       <c r="C722">
-        <v>140</v>
+        <v>30</v>
       </c>
       <c r="D722" t="str">
-        <v>Swiggy</v>
+        <v>Water</v>
       </c>
     </row>
     <row r="723">
       <c r="A723" t="str">
-        <v>2021-12-15</v>
+        <v>2021-11-23</v>
       </c>
       <c r="B723" t="str">
-        <v>Food</v>
+        <v>Bills</v>
       </c>
       <c r="C723">
-        <v>30</v>
+        <v>589</v>
       </c>
       <c r="D723" t="str">
-        <v>Water</v>
+        <v>Airtel Wifi Mainpuri</v>
       </c>
     </row>
     <row r="724">
       <c r="A724" t="str">
-        <v>2021-11-23</v>
+        <v>2021-10-23</v>
       </c>
       <c r="B724" t="str">
         <v>Bills</v>
       </c>
       <c r="C724">
-        <v>589</v>
+        <v>439</v>
       </c>
       <c r="D724" t="str">
-        <v>Airtel Wifi Mainpuri</v>
+        <v>Airtel Wifi</v>
       </c>
     </row>
     <row r="725">
       <c r="A725" t="str">
-        <v>2021-10-23</v>
+        <v>2021-12-10</v>
       </c>
       <c r="B725" t="str">
-        <v>Bills</v>
+        <v>Food</v>
       </c>
       <c r="C725">
-        <v>439</v>
+        <v>151</v>
       </c>
       <c r="D725" t="str">
-        <v>Airtel Wifi</v>
+        <v>Water And Dairy</v>
       </c>
     </row>
     <row r="726">
       <c r="A726" t="str">
-        <v>2021-12-10</v>
+        <v>2021-12-22</v>
       </c>
       <c r="B726" t="str">
         <v>Food</v>
       </c>
       <c r="C726">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D726" t="str">
-        <v>Water And Dairy</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="727">
       <c r="A727" t="str">
-        <v>2021-12-22</v>
+        <v>2021-10-26</v>
       </c>
       <c r="B727" t="str">
-        <v>Food</v>
+        <v>Other Income</v>
       </c>
       <c r="C727">
-        <v>149</v>
+        <v>35240</v>
       </c>
       <c r="D727" t="str">
-        <v>Swiggy</v>
+        <v>Refund ITR</v>
       </c>
     </row>
     <row r="728">
@@ -10476,122 +10476,122 @@
         <v>2021-10-26</v>
       </c>
       <c r="B728" t="str">
-        <v>Other Income</v>
+        <v>Food</v>
       </c>
       <c r="C728">
-        <v>35240</v>
+        <v>109</v>
       </c>
       <c r="D728" t="str">
-        <v>Refund ITR</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="729">
       <c r="A729" t="str">
-        <v>2021-10-26</v>
+        <v>2021-10-20</v>
       </c>
       <c r="B729" t="str">
         <v>Food</v>
       </c>
       <c r="C729">
-        <v>109</v>
+        <v>280</v>
       </c>
       <c r="D729" t="str">
-        <v>Swiggy</v>
+        <v>Bigbasket</v>
       </c>
     </row>
     <row r="730">
       <c r="A730" t="str">
-        <v>2021-10-20</v>
+        <v>2021-12-19</v>
       </c>
       <c r="B730" t="str">
         <v>Food</v>
       </c>
       <c r="C730">
-        <v>280</v>
+        <v>131</v>
       </c>
       <c r="D730" t="str">
-        <v>Bigbasket</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="731">
       <c r="A731" t="str">
-        <v>2021-12-19</v>
+        <v>2021-10-20</v>
       </c>
       <c r="B731" t="str">
         <v>Food</v>
       </c>
       <c r="C731">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="D731" t="str">
-        <v>Swiggy</v>
+        <v>Water and Dairy</v>
       </c>
     </row>
     <row r="732">
       <c r="A732" t="str">
-        <v>2021-10-20</v>
+        <v>2021-12-23</v>
       </c>
       <c r="B732" t="str">
-        <v>Food</v>
+        <v>Entertainment</v>
       </c>
       <c r="C732">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="D732" t="str">
-        <v>Water and Dairy</v>
+        <v>Netflix</v>
       </c>
     </row>
     <row r="733">
       <c r="A733" t="str">
-        <v>2021-12-23</v>
+        <v>2021-12-03</v>
       </c>
       <c r="B733" t="str">
-        <v>Entertainment</v>
+        <v>Transportation</v>
       </c>
       <c r="C733">
-        <v>149</v>
+        <v>530</v>
       </c>
       <c r="D733" t="str">
-        <v>Netflix</v>
+        <v>Irctc To Delhi</v>
       </c>
     </row>
     <row r="734">
       <c r="A734" t="str">
-        <v>2021-12-03</v>
+        <v>2021-10-18</v>
       </c>
       <c r="B734" t="str">
-        <v>Transportation</v>
+        <v>Food</v>
       </c>
       <c r="C734">
-        <v>530</v>
+        <v>150</v>
       </c>
       <c r="D734" t="str">
-        <v>Irctc To Delhi</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="735">
       <c r="A735" t="str">
-        <v>2021-10-18</v>
+        <v>2021-12-08</v>
       </c>
       <c r="B735" t="str">
-        <v>Food</v>
+        <v>Salary</v>
       </c>
       <c r="C735">
-        <v>150</v>
-      </c>
-      <c r="D735" t="str">
-        <v>Swiggy</v>
+        <v>61500</v>
       </c>
     </row>
     <row r="736">
       <c r="A736" t="str">
-        <v>2021-12-08</v>
+        <v>2021-12-05</v>
       </c>
       <c r="B736" t="str">
-        <v>Salary</v>
+        <v>Transportation</v>
       </c>
       <c r="C736">
-        <v>61500</v>
+        <v>350</v>
+      </c>
+      <c r="D736" t="str">
+        <v>Ola Auto</v>
       </c>
     </row>
     <row r="737">
@@ -10599,164 +10599,164 @@
         <v>2021-12-05</v>
       </c>
       <c r="B737" t="str">
-        <v>Transportation</v>
+        <v>Food</v>
       </c>
       <c r="C737">
-        <v>350</v>
+        <v>88</v>
       </c>
       <c r="D737" t="str">
-        <v>Ola Auto</v>
+        <v>Water And Dairy</v>
       </c>
     </row>
     <row r="738">
       <c r="A738" t="str">
-        <v>2021-12-05</v>
+        <v>2021-10-29</v>
       </c>
       <c r="B738" t="str">
         <v>Food</v>
       </c>
       <c r="C738">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="D738" t="str">
-        <v>Water And Dairy</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="739">
       <c r="A739" t="str">
-        <v>2021-10-29</v>
+        <v>2021-11-27</v>
       </c>
       <c r="B739" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C739">
-        <v>109</v>
+        <v>704</v>
       </c>
       <c r="D739" t="str">
-        <v>Swiggy</v>
+        <v>Bulbs Amazon</v>
       </c>
     </row>
     <row r="740">
       <c r="A740" t="str">
-        <v>2021-11-27</v>
+        <v>2021-10-22</v>
       </c>
       <c r="B740" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C740">
-        <v>704</v>
+        <v>130</v>
       </c>
       <c r="D740" t="str">
-        <v>Bulbs Amazon</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="741">
       <c r="A741" t="str">
-        <v>2021-10-22</v>
+        <v>2021-10-28</v>
       </c>
       <c r="B741" t="str">
         <v>Food</v>
       </c>
       <c r="C741">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="D741" t="str">
-        <v>Swiggy</v>
+        <v>Water</v>
       </c>
     </row>
     <row r="742">
       <c r="A742" t="str">
-        <v>2021-10-28</v>
+        <v>2021-11-03</v>
       </c>
       <c r="B742" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C742">
-        <v>30</v>
+        <v>11799</v>
       </c>
       <c r="D742" t="str">
-        <v>Water</v>
+        <v>Monitor</v>
       </c>
     </row>
     <row r="743">
       <c r="A743" t="str">
-        <v>2021-11-03</v>
+        <v>2021-12-20</v>
       </c>
       <c r="B743" t="str">
-        <v>Shopping</v>
+        <v>Home</v>
       </c>
       <c r="C743">
-        <v>11799</v>
+        <v>120</v>
       </c>
       <c r="D743" t="str">
-        <v>Monitor</v>
+        <v>Garbage</v>
       </c>
     </row>
     <row r="744">
       <c r="A744" t="str">
-        <v>2021-12-20</v>
+        <v>2021-11-29</v>
       </c>
       <c r="B744" t="str">
-        <v>Home</v>
+        <v>Other Income</v>
       </c>
       <c r="C744">
-        <v>120</v>
+        <v>705</v>
       </c>
       <c r="D744" t="str">
-        <v>Garbage</v>
+        <v>Amazon Pay Cashback</v>
       </c>
     </row>
     <row r="745">
       <c r="A745" t="str">
-        <v>2021-11-29</v>
+        <v>2021-10-26</v>
       </c>
       <c r="B745" t="str">
-        <v>Other Income</v>
+        <v>Food</v>
       </c>
       <c r="C745">
-        <v>705</v>
+        <v>194</v>
       </c>
       <c r="D745" t="str">
-        <v>Amazon Pay Cashback</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="746">
       <c r="A746" t="str">
-        <v>2021-10-26</v>
+        <v>2021-11-27</v>
       </c>
       <c r="B746" t="str">
-        <v>Food</v>
+        <v>Transportation</v>
       </c>
       <c r="C746">
-        <v>194</v>
+        <v>80</v>
       </c>
       <c r="D746" t="str">
-        <v>Swiggy</v>
+        <v>Rikshaw</v>
       </c>
     </row>
     <row r="747">
       <c r="A747" t="str">
-        <v>2021-11-27</v>
+        <v>2021-12-10</v>
       </c>
       <c r="B747" t="str">
-        <v>Transportation</v>
+        <v>Food</v>
       </c>
       <c r="C747">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="D747" t="str">
-        <v>Rikshaw</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="748">
       <c r="A748" t="str">
-        <v>2021-12-10</v>
+        <v>2021-12-09</v>
       </c>
       <c r="B748" t="str">
         <v>Food</v>
       </c>
       <c r="C748">
-        <v>109</v>
+        <v>154</v>
       </c>
       <c r="D748" t="str">
         <v>Swiggy</v>
@@ -10764,100 +10764,100 @@
     </row>
     <row r="749">
       <c r="A749" t="str">
-        <v>2021-12-09</v>
+        <v>2021-12-21</v>
       </c>
       <c r="B749" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C749">
-        <v>154</v>
+        <v>856</v>
       </c>
       <c r="D749" t="str">
-        <v>Swiggy</v>
+        <v>Amazon</v>
       </c>
     </row>
     <row r="750">
       <c r="A750" t="str">
-        <v>2021-12-21</v>
+        <v>2021-12-01</v>
       </c>
       <c r="B750" t="str">
         <v>Shopping</v>
       </c>
       <c r="C750">
-        <v>856</v>
+        <v>1558</v>
       </c>
       <c r="D750" t="str">
-        <v>Amazon</v>
+        <v>Flipkart Water Taps</v>
       </c>
     </row>
     <row r="751">
       <c r="A751" t="str">
-        <v>2021-12-01</v>
+        <v>2021-12-05</v>
       </c>
       <c r="B751" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C751">
-        <v>1558</v>
+        <v>1198</v>
       </c>
       <c r="D751" t="str">
-        <v>Flipkart Water Taps</v>
+        <v>Bigbasket</v>
       </c>
     </row>
     <row r="752">
       <c r="A752" t="str">
-        <v>2021-12-05</v>
+        <v>2021-11-28</v>
       </c>
       <c r="B752" t="str">
-        <v>Food</v>
+        <v>Entertainment</v>
       </c>
       <c r="C752">
-        <v>1198</v>
+        <v>119</v>
       </c>
       <c r="D752" t="str">
-        <v>Bigbasket</v>
+        <v>Spotify</v>
       </c>
     </row>
     <row r="753">
       <c r="A753" t="str">
-        <v>2021-11-28</v>
+        <v>2021-12-23</v>
       </c>
       <c r="B753" t="str">
-        <v>Entertainment</v>
+        <v>Bills</v>
       </c>
       <c r="C753">
-        <v>119</v>
+        <v>589</v>
       </c>
       <c r="D753" t="str">
-        <v>Spotify</v>
+        <v>Airtel Wifi Mainpuri</v>
       </c>
     </row>
     <row r="754">
       <c r="A754" t="str">
-        <v>2021-12-23</v>
+        <v>2021-12-06</v>
       </c>
       <c r="B754" t="str">
-        <v>Bills</v>
+        <v>Home</v>
       </c>
       <c r="C754">
-        <v>589</v>
+        <v>400</v>
       </c>
       <c r="D754" t="str">
-        <v>Airtel Wifi Mainpuri</v>
+        <v>Maintenance</v>
       </c>
     </row>
     <row r="755">
       <c r="A755" t="str">
-        <v>2021-12-06</v>
+        <v>2021-12-13</v>
       </c>
       <c r="B755" t="str">
-        <v>Home</v>
+        <v>Shopping</v>
       </c>
       <c r="C755">
-        <v>400</v>
+        <v>3500</v>
       </c>
       <c r="D755" t="str">
-        <v>Maintenance</v>
+        <v>Laptop Battery</v>
       </c>
     </row>
     <row r="756">
@@ -10865,24 +10865,24 @@
         <v>2021-12-13</v>
       </c>
       <c r="B756" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C756">
-        <v>3500</v>
+        <v>184</v>
       </c>
       <c r="D756" t="str">
-        <v>Laptop Battery</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="757">
       <c r="A757" t="str">
-        <v>2021-12-13</v>
+        <v>2021-12-20</v>
       </c>
       <c r="B757" t="str">
         <v>Food</v>
       </c>
       <c r="C757">
-        <v>184</v>
+        <v>153</v>
       </c>
       <c r="D757" t="str">
         <v>Swiggy</v>
@@ -10890,13 +10890,13 @@
     </row>
     <row r="758">
       <c r="A758" t="str">
-        <v>2021-12-20</v>
+        <v>2022-01-01</v>
       </c>
       <c r="B758" t="str">
         <v>Food</v>
       </c>
       <c r="C758">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="D758" t="str">
         <v>Swiggy</v>
@@ -10904,360 +10904,360 @@
     </row>
     <row r="759">
       <c r="A759" t="str">
-        <v>2022-01-01</v>
+        <v>2022-01-18</v>
       </c>
       <c r="B759" t="str">
-        <v>Food</v>
+        <v>Home</v>
       </c>
       <c r="C759">
-        <v>121</v>
+        <v>9000</v>
       </c>
       <c r="D759" t="str">
-        <v>Swiggy</v>
+        <v>Rent</v>
       </c>
     </row>
     <row r="760">
       <c r="A760" t="str">
-        <v>2022-01-18</v>
+        <v>2021-12-25</v>
       </c>
       <c r="B760" t="str">
-        <v>Home</v>
+        <v>Food</v>
       </c>
       <c r="C760">
-        <v>9000</v>
+        <v>264</v>
       </c>
       <c r="D760" t="str">
-        <v>Rent</v>
+        <v>Water And Dairy</v>
       </c>
     </row>
     <row r="761">
       <c r="A761" t="str">
-        <v>2021-12-25</v>
+        <v>2021-12-30</v>
       </c>
       <c r="B761" t="str">
-        <v>Food</v>
+        <v>Other Income</v>
       </c>
       <c r="C761">
-        <v>264</v>
+        <v>1000</v>
       </c>
       <c r="D761" t="str">
-        <v>Water And Dairy</v>
+        <v>MDS Swiggy Coupon</v>
       </c>
     </row>
     <row r="762">
       <c r="A762" t="str">
-        <v>2021-12-30</v>
+        <v>2022-01-08</v>
       </c>
       <c r="B762" t="str">
-        <v>Other Income</v>
+        <v>Home</v>
       </c>
       <c r="C762">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="D762" t="str">
-        <v>MDS Swiggy Coupon</v>
+        <v>Maintenance</v>
       </c>
     </row>
     <row r="763">
       <c r="A763" t="str">
-        <v>2022-01-08</v>
+        <v>2022-01-06</v>
       </c>
       <c r="B763" t="str">
-        <v>Home</v>
+        <v>Salary</v>
       </c>
       <c r="C763">
-        <v>200</v>
-      </c>
-      <c r="D763" t="str">
-        <v>Maintenance</v>
+        <v>75725</v>
       </c>
     </row>
     <row r="764">
       <c r="A764" t="str">
-        <v>2022-01-06</v>
+        <v>2021-12-10</v>
       </c>
       <c r="B764" t="str">
-        <v>Salary</v>
+        <v>Shopping</v>
       </c>
       <c r="C764">
-        <v>75725</v>
+        <v>568</v>
+      </c>
+      <c r="D764" t="str">
+        <v>Amazon</v>
       </c>
     </row>
     <row r="765">
       <c r="A765" t="str">
-        <v>2021-12-10</v>
+        <v>2022-01-04</v>
       </c>
       <c r="B765" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C765">
-        <v>568</v>
+        <v>88</v>
       </c>
       <c r="D765" t="str">
-        <v>Amazon</v>
+        <v>Dairy And Water</v>
       </c>
     </row>
     <row r="766">
       <c r="A766" t="str">
-        <v>2022-01-04</v>
+        <v>2022-01-27</v>
       </c>
       <c r="B766" t="str">
-        <v>Food</v>
+        <v>Bills</v>
       </c>
       <c r="C766">
-        <v>88</v>
+        <v>589</v>
       </c>
       <c r="D766" t="str">
-        <v>Dairy And Water</v>
+        <v>Airtel Wifi</v>
       </c>
     </row>
     <row r="767">
       <c r="A767" t="str">
-        <v>2022-01-27</v>
+        <v>2022-01-18</v>
       </c>
       <c r="B767" t="str">
-        <v>Bills</v>
+        <v>Food</v>
       </c>
       <c r="C767">
-        <v>589</v>
+        <v>163</v>
       </c>
       <c r="D767" t="str">
-        <v>Airtel Wifi</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="768">
       <c r="A768" t="str">
-        <v>2022-01-18</v>
+        <v>2021-12-28</v>
       </c>
       <c r="B768" t="str">
-        <v>Food</v>
+        <v>Bills</v>
       </c>
       <c r="C768">
-        <v>163</v>
+        <v>589</v>
       </c>
       <c r="D768" t="str">
-        <v>Swiggy</v>
+        <v>Airtel Wifi</v>
       </c>
     </row>
     <row r="769">
       <c r="A769" t="str">
-        <v>2021-12-28</v>
+        <v>2021-12-12</v>
       </c>
       <c r="B769" t="str">
-        <v>Bills</v>
+        <v>Entertainment</v>
       </c>
       <c r="C769">
-        <v>589</v>
+        <v>999</v>
       </c>
       <c r="D769" t="str">
-        <v>Airtel Wifi</v>
+        <v>Prime</v>
       </c>
     </row>
     <row r="770">
       <c r="A770" t="str">
-        <v>2021-12-12</v>
+        <v>2022-01-12</v>
       </c>
       <c r="B770" t="str">
-        <v>Entertainment</v>
+        <v>Food</v>
       </c>
       <c r="C770">
-        <v>999</v>
+        <v>311</v>
       </c>
       <c r="D770" t="str">
-        <v>Prime</v>
+        <v>Grofers</v>
       </c>
     </row>
     <row r="771">
       <c r="A771" t="str">
-        <v>2022-01-12</v>
+        <v>2022-01-09</v>
       </c>
       <c r="B771" t="str">
         <v>Food</v>
       </c>
       <c r="C771">
-        <v>311</v>
+        <v>63</v>
       </c>
       <c r="D771" t="str">
-        <v>Grofers</v>
+        <v>Dairy</v>
       </c>
     </row>
     <row r="772">
       <c r="A772" t="str">
-        <v>2022-01-09</v>
+        <v>2021-12-31</v>
       </c>
       <c r="B772" t="str">
-        <v>Food</v>
+        <v>Entertainment</v>
       </c>
       <c r="C772">
-        <v>63</v>
+        <v>129</v>
       </c>
       <c r="D772" t="str">
-        <v>Dairy</v>
+        <v>YouTube</v>
       </c>
     </row>
     <row r="773">
       <c r="A773" t="str">
-        <v>2021-12-31</v>
+        <v>2022-01-08</v>
       </c>
       <c r="B773" t="str">
-        <v>Entertainment</v>
+        <v>Food</v>
       </c>
       <c r="C773">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D773" t="str">
-        <v>YouTube</v>
+        <v>Water and Dairy</v>
       </c>
     </row>
     <row r="774">
       <c r="A774" t="str">
-        <v>2022-01-08</v>
+        <v>2021-12-25</v>
       </c>
       <c r="B774" t="str">
-        <v>Food</v>
+        <v>Bills</v>
       </c>
       <c r="C774">
-        <v>123</v>
+        <v>1799</v>
       </c>
       <c r="D774" t="str">
-        <v>Water and Dairy</v>
+        <v>Airtel Full Year Plan</v>
       </c>
     </row>
     <row r="775">
       <c r="A775" t="str">
-        <v>2021-12-25</v>
+        <v>2022-01-16</v>
       </c>
       <c r="B775" t="str">
-        <v>Bills</v>
+        <v>Food</v>
       </c>
       <c r="C775">
-        <v>1799</v>
+        <v>768</v>
       </c>
       <c r="D775" t="str">
-        <v>Airtel Full Year Plan</v>
+        <v>Grofers (Blinkit)</v>
       </c>
     </row>
     <row r="776">
       <c r="A776" t="str">
-        <v>2022-01-16</v>
+        <v>2022-01-20</v>
       </c>
       <c r="B776" t="str">
         <v>Food</v>
       </c>
       <c r="C776">
-        <v>768</v>
+        <v>155</v>
       </c>
       <c r="D776" t="str">
-        <v>Grofers (Blinkit)</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="777">
       <c r="A777" t="str">
-        <v>2022-01-20</v>
+        <v>2022-01-22</v>
       </c>
       <c r="B777" t="str">
-        <v>Food</v>
+        <v>Transportation</v>
       </c>
       <c r="C777">
-        <v>155</v>
+        <v>340</v>
       </c>
       <c r="D777" t="str">
-        <v>Swiggy</v>
+        <v>Bike Service</v>
       </c>
     </row>
     <row r="778">
       <c r="A778" t="str">
-        <v>2022-01-22</v>
+        <v>2022-02-07</v>
       </c>
       <c r="B778" t="str">
-        <v>Transportation</v>
+        <v>Food</v>
       </c>
       <c r="C778">
-        <v>340</v>
+        <v>214</v>
       </c>
       <c r="D778" t="str">
-        <v>Bike Service</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="779">
       <c r="A779" t="str">
-        <v>2022-02-07</v>
+        <v>2022-01-08</v>
       </c>
       <c r="B779" t="str">
         <v>Food</v>
       </c>
       <c r="C779">
-        <v>214</v>
+        <v>1492</v>
       </c>
       <c r="D779" t="str">
-        <v>Swiggy</v>
+        <v>Grofers (Blinkit)</v>
       </c>
     </row>
     <row r="780">
       <c r="A780" t="str">
-        <v>2022-01-08</v>
+        <v>2021-12-28</v>
       </c>
       <c r="B780" t="str">
         <v>Food</v>
       </c>
       <c r="C780">
-        <v>1492</v>
+        <v>494</v>
       </c>
       <c r="D780" t="str">
-        <v>Grofers (Blinkit)</v>
+        <v>Bigbasket</v>
       </c>
     </row>
     <row r="781">
       <c r="A781" t="str">
-        <v>2021-12-28</v>
+        <v>2022-01-21</v>
       </c>
       <c r="B781" t="str">
         <v>Food</v>
       </c>
       <c r="C781">
-        <v>494</v>
+        <v>148</v>
       </c>
       <c r="D781" t="str">
-        <v>Bigbasket</v>
+        <v>Water And Dairy</v>
       </c>
     </row>
     <row r="782">
       <c r="A782" t="str">
-        <v>2022-01-21</v>
+        <v>2021-12-23</v>
       </c>
       <c r="B782" t="str">
-        <v>Food</v>
+        <v>Bills</v>
       </c>
       <c r="C782">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="D782" t="str">
-        <v>Water And Dairy</v>
+        <v>Airtel Recharge</v>
       </c>
     </row>
     <row r="783">
       <c r="A783" t="str">
-        <v>2021-12-23</v>
+        <v>2022-01-11</v>
       </c>
       <c r="B783" t="str">
-        <v>Bills</v>
+        <v>Food</v>
       </c>
       <c r="C783">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="D783" t="str">
-        <v>Airtel Recharge</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="784">
       <c r="A784" t="str">
-        <v>2022-01-11</v>
+        <v>2021-12-17</v>
       </c>
       <c r="B784" t="str">
         <v>Food</v>
       </c>
       <c r="C784">
-        <v>149</v>
+        <v>194</v>
       </c>
       <c r="D784" t="str">
         <v>Swiggy</v>
@@ -11265,35 +11265,35 @@
     </row>
     <row r="785">
       <c r="A785" t="str">
-        <v>2021-12-17</v>
+        <v>2021-12-28</v>
       </c>
       <c r="B785" t="str">
         <v>Food</v>
       </c>
       <c r="C785">
-        <v>194</v>
+        <v>120</v>
       </c>
       <c r="D785" t="str">
-        <v>Swiggy</v>
+        <v>Zomato</v>
       </c>
     </row>
     <row r="786">
       <c r="A786" t="str">
-        <v>2021-12-28</v>
+        <v>2022-01-10</v>
       </c>
       <c r="B786" t="str">
         <v>Food</v>
       </c>
       <c r="C786">
-        <v>120</v>
+        <v>226</v>
       </c>
       <c r="D786" t="str">
-        <v>Zomato</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="787">
       <c r="A787" t="str">
-        <v>2022-01-10</v>
+        <v>2021-12-31</v>
       </c>
       <c r="B787" t="str">
         <v>Food</v>
@@ -11307,13 +11307,13 @@
     </row>
     <row r="788">
       <c r="A788" t="str">
-        <v>2021-12-31</v>
+        <v>2021-12-27</v>
       </c>
       <c r="B788" t="str">
         <v>Food</v>
       </c>
       <c r="C788">
-        <v>226</v>
+        <v>130</v>
       </c>
       <c r="D788" t="str">
         <v>Swiggy</v>
@@ -11321,41 +11321,41 @@
     </row>
     <row r="789">
       <c r="A789" t="str">
-        <v>2021-12-27</v>
+        <v>2022-01-16</v>
       </c>
       <c r="B789" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C789">
-        <v>130</v>
+        <v>273</v>
       </c>
       <c r="D789" t="str">
-        <v>Swiggy</v>
+        <v>Hand Juicer</v>
       </c>
     </row>
     <row r="790">
       <c r="A790" t="str">
-        <v>2022-01-16</v>
+        <v>2021-12-31</v>
       </c>
       <c r="B790" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C790">
-        <v>273</v>
+        <v>729</v>
       </c>
       <c r="D790" t="str">
-        <v>Hand Juicer</v>
+        <v>Bigbasket</v>
       </c>
     </row>
     <row r="791">
       <c r="A791" t="str">
-        <v>2021-12-31</v>
+        <v>2021-12-11</v>
       </c>
       <c r="B791" t="str">
         <v>Food</v>
       </c>
       <c r="C791">
-        <v>729</v>
+        <v>735</v>
       </c>
       <c r="D791" t="str">
         <v>Bigbasket</v>
@@ -11363,142 +11363,142 @@
     </row>
     <row r="792">
       <c r="A792" t="str">
-        <v>2021-12-11</v>
+        <v>2021-12-01</v>
       </c>
       <c r="B792" t="str">
-        <v>Food</v>
+        <v>Entertainment</v>
       </c>
       <c r="C792">
-        <v>735</v>
+        <v>129</v>
       </c>
       <c r="D792" t="str">
-        <v>Bigbasket</v>
+        <v>YouTube</v>
       </c>
     </row>
     <row r="793">
       <c r="A793" t="str">
-        <v>2021-12-01</v>
+        <v>2021-12-29</v>
       </c>
       <c r="B793" t="str">
-        <v>Entertainment</v>
+        <v>Food</v>
       </c>
       <c r="C793">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="D793" t="str">
-        <v>YouTube</v>
+        <v>Dairy</v>
       </c>
     </row>
     <row r="794">
       <c r="A794" t="str">
-        <v>2021-12-29</v>
+        <v>2022-01-22</v>
       </c>
       <c r="B794" t="str">
         <v>Food</v>
       </c>
       <c r="C794">
-        <v>58</v>
+        <v>1396</v>
       </c>
       <c r="D794" t="str">
-        <v>Dairy</v>
+        <v>Blinkit (Grofers)</v>
       </c>
     </row>
     <row r="795">
       <c r="A795" t="str">
-        <v>2022-01-22</v>
+        <v>2021-12-08</v>
       </c>
       <c r="B795" t="str">
         <v>Food</v>
       </c>
       <c r="C795">
-        <v>1396</v>
+        <v>158</v>
       </c>
       <c r="D795" t="str">
-        <v>Blinkit (Grofers)</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="796">
       <c r="A796" t="str">
-        <v>2021-12-08</v>
+        <v>2021-12-17</v>
       </c>
       <c r="B796" t="str">
-        <v>Food</v>
+        <v>Home</v>
       </c>
       <c r="C796">
-        <v>158</v>
+        <v>9000</v>
       </c>
       <c r="D796" t="str">
-        <v>Swiggy</v>
+        <v>Rent</v>
       </c>
     </row>
     <row r="797">
       <c r="A797" t="str">
-        <v>2021-12-17</v>
+        <v>2021-12-10</v>
       </c>
       <c r="B797" t="str">
-        <v>Home</v>
+        <v>Bills</v>
       </c>
       <c r="C797">
-        <v>9000</v>
+        <v>3200</v>
       </c>
       <c r="D797" t="str">
-        <v>Rent</v>
+        <v>Water Bill Aug 19 to Jan 20</v>
       </c>
     </row>
     <row r="798">
       <c r="A798" t="str">
-        <v>2021-12-10</v>
+        <v>2022-02-02</v>
       </c>
       <c r="B798" t="str">
-        <v>Bills</v>
+        <v>Food</v>
       </c>
       <c r="C798">
-        <v>3200</v>
+        <v>143</v>
       </c>
       <c r="D798" t="str">
-        <v>Water Bill Aug 19 to Jan 20</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="799">
       <c r="A799" t="str">
-        <v>2022-02-02</v>
+        <v>2022-02-01</v>
       </c>
       <c r="B799" t="str">
-        <v>Food</v>
+        <v>Entertainment</v>
       </c>
       <c r="C799">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="D799" t="str">
-        <v>Swiggy</v>
+        <v>YouTube Premium</v>
       </c>
     </row>
     <row r="800">
       <c r="A800" t="str">
-        <v>2022-02-01</v>
+        <v>2021-12-31</v>
       </c>
       <c r="B800" t="str">
-        <v>Entertainment</v>
+        <v>Other Income</v>
       </c>
       <c r="C800">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="D800" t="str">
-        <v>YouTube Premium</v>
+        <v>Amazon Cashback</v>
       </c>
     </row>
     <row r="801">
       <c r="A801" t="str">
-        <v>2021-12-31</v>
+        <v>2022-01-25</v>
       </c>
       <c r="B801" t="str">
-        <v>Other Income</v>
+        <v>Food</v>
       </c>
       <c r="C801">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D801" t="str">
-        <v>Amazon Cashback</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="802">
@@ -11509,7 +11509,7 @@
         <v>Food</v>
       </c>
       <c r="C802">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D802" t="str">
         <v>Swiggy</v>
@@ -11517,13 +11517,13 @@
     </row>
     <row r="803">
       <c r="A803" t="str">
-        <v>2022-01-25</v>
+        <v>2022-01-21</v>
       </c>
       <c r="B803" t="str">
         <v>Food</v>
       </c>
       <c r="C803">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D803" t="str">
         <v>Swiggy</v>
@@ -11531,83 +11531,83 @@
     </row>
     <row r="804">
       <c r="A804" t="str">
-        <v>2022-01-21</v>
+        <v>2021-12-12</v>
       </c>
       <c r="B804" t="str">
         <v>Food</v>
       </c>
       <c r="C804">
-        <v>138</v>
+        <v>578</v>
       </c>
       <c r="D804" t="str">
-        <v>Swiggy</v>
+        <v>Bigbasket</v>
       </c>
     </row>
     <row r="805">
       <c r="A805" t="str">
-        <v>2021-12-12</v>
+        <v>2021-12-28</v>
       </c>
       <c r="B805" t="str">
-        <v>Food</v>
+        <v>Entertainment</v>
       </c>
       <c r="C805">
-        <v>578</v>
+        <v>119</v>
       </c>
       <c r="D805" t="str">
-        <v>Bigbasket</v>
+        <v>Spotify</v>
       </c>
     </row>
     <row r="806">
       <c r="A806" t="str">
-        <v>2021-12-28</v>
+        <v>2022-01-26</v>
       </c>
       <c r="B806" t="str">
-        <v>Entertainment</v>
+        <v>Food</v>
       </c>
       <c r="C806">
-        <v>119</v>
+        <v>407</v>
       </c>
       <c r="D806" t="str">
-        <v>Spotify</v>
+        <v>Grofers (Blinkit)</v>
       </c>
     </row>
     <row r="807">
       <c r="A807" t="str">
-        <v>2022-01-26</v>
+        <v>2022-01-16</v>
       </c>
       <c r="B807" t="str">
-        <v>Food</v>
+        <v>Home</v>
       </c>
       <c r="C807">
-        <v>407</v>
+        <v>60</v>
       </c>
       <c r="D807" t="str">
-        <v>Grofers (Blinkit)</v>
+        <v>Garbage</v>
       </c>
     </row>
     <row r="808">
       <c r="A808" t="str">
-        <v>2022-01-16</v>
+        <v>2021-12-28</v>
       </c>
       <c r="B808" t="str">
-        <v>Home</v>
+        <v>Food</v>
       </c>
       <c r="C808">
-        <v>60</v>
+        <v>137</v>
       </c>
       <c r="D808" t="str">
-        <v>Garbage</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="809">
       <c r="A809" t="str">
-        <v>2021-12-28</v>
+        <v>2021-12-31</v>
       </c>
       <c r="B809" t="str">
         <v>Food</v>
       </c>
       <c r="C809">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="D809" t="str">
         <v>Swiggy</v>
@@ -11615,41 +11615,41 @@
     </row>
     <row r="810">
       <c r="A810" t="str">
-        <v>2021-12-31</v>
+        <v>2022-01-24</v>
       </c>
       <c r="B810" t="str">
-        <v>Food</v>
+        <v>Bills</v>
       </c>
       <c r="C810">
-        <v>120</v>
+        <v>589</v>
       </c>
       <c r="D810" t="str">
-        <v>Swiggy</v>
+        <v>Airtel Wifi Mainpuri</v>
       </c>
     </row>
     <row r="811">
       <c r="A811" t="str">
-        <v>2022-01-24</v>
+        <v>2022-02-01</v>
       </c>
       <c r="B811" t="str">
-        <v>Bills</v>
+        <v>Food</v>
       </c>
       <c r="C811">
-        <v>589</v>
+        <v>138</v>
       </c>
       <c r="D811" t="str">
-        <v>Airtel Wifi Mainpuri</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="812">
       <c r="A812" t="str">
-        <v>2022-02-01</v>
+        <v>2022-01-29</v>
       </c>
       <c r="B812" t="str">
         <v>Food</v>
       </c>
       <c r="C812">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="D812" t="str">
         <v>Swiggy</v>
@@ -11657,13 +11657,13 @@
     </row>
     <row r="813">
       <c r="A813" t="str">
-        <v>2022-01-29</v>
+        <v>2022-02-03</v>
       </c>
       <c r="B813" t="str">
         <v>Food</v>
       </c>
       <c r="C813">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="D813" t="str">
         <v>Swiggy</v>
@@ -11671,74 +11671,74 @@
     </row>
     <row r="814">
       <c r="A814" t="str">
-        <v>2022-02-03</v>
+        <v>2022-02-05</v>
       </c>
       <c r="B814" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C814">
-        <v>158</v>
+        <v>298</v>
       </c>
       <c r="D814" t="str">
-        <v>Swiggy</v>
+        <v>Urban Company Haircut</v>
       </c>
     </row>
     <row r="815">
       <c r="A815" t="str">
-        <v>2022-02-05</v>
+        <v>2022-02-11</v>
       </c>
       <c r="B815" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C815">
-        <v>298</v>
+        <v>164</v>
       </c>
       <c r="D815" t="str">
-        <v>Urban Company Haircut</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="816">
       <c r="A816" t="str">
-        <v>2022-02-11</v>
+        <v>2022-02-04</v>
       </c>
       <c r="B816" t="str">
         <v>Food</v>
       </c>
       <c r="C816">
-        <v>164</v>
+        <v>1550</v>
       </c>
       <c r="D816" t="str">
-        <v>Swiggy</v>
+        <v>Blinkit (Grofers)</v>
       </c>
     </row>
     <row r="817">
       <c r="A817" t="str">
-        <v>2022-02-04</v>
+        <v>2022-02-05</v>
       </c>
       <c r="B817" t="str">
-        <v>Food</v>
+        <v>Salary</v>
       </c>
       <c r="C817">
-        <v>1550</v>
-      </c>
-      <c r="D817" t="str">
-        <v>Blinkit (Grofers)</v>
+        <v>86520</v>
       </c>
     </row>
     <row r="818">
       <c r="A818" t="str">
-        <v>2022-02-05</v>
+        <v>2022-02-12</v>
       </c>
       <c r="B818" t="str">
-        <v>Salary</v>
+        <v>Food</v>
       </c>
       <c r="C818">
-        <v>86520</v>
+        <v>30</v>
+      </c>
+      <c r="D818" t="str">
+        <v>Water</v>
       </c>
     </row>
     <row r="819">
       <c r="A819" t="str">
-        <v>2022-02-12</v>
+        <v>2022-01-28</v>
       </c>
       <c r="B819" t="str">
         <v>Food</v>
@@ -11752,114 +11752,114 @@
     </row>
     <row r="820">
       <c r="A820" t="str">
-        <v>2022-01-28</v>
+        <v>2022-02-12</v>
       </c>
       <c r="B820" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C820">
-        <v>30</v>
+        <v>7990</v>
       </c>
       <c r="D820" t="str">
-        <v>Water</v>
+        <v>Green Soul Chair</v>
       </c>
     </row>
     <row r="821">
       <c r="A821" t="str">
-        <v>2022-02-12</v>
+        <v>2022-02-05</v>
       </c>
       <c r="B821" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C821">
-        <v>7990</v>
+        <v>338</v>
       </c>
       <c r="D821" t="str">
-        <v>Green Soul Chair</v>
+        <v>Blinkit</v>
       </c>
     </row>
     <row r="822">
       <c r="A822" t="str">
-        <v>2022-02-05</v>
+        <v>2022-02-09</v>
       </c>
       <c r="B822" t="str">
         <v>Food</v>
       </c>
       <c r="C822">
-        <v>338</v>
+        <v>143</v>
       </c>
       <c r="D822" t="str">
-        <v>Blinkit</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="823">
       <c r="A823" t="str">
-        <v>2022-02-09</v>
+        <v>2022-01-29</v>
       </c>
       <c r="B823" t="str">
-        <v>Food</v>
+        <v>Transportation</v>
       </c>
       <c r="C823">
-        <v>143</v>
+        <v>950</v>
       </c>
       <c r="D823" t="str">
-        <v>Swiggy</v>
+        <v>Bike's New Battery</v>
       </c>
     </row>
     <row r="824">
       <c r="A824" t="str">
-        <v>2022-01-29</v>
+        <v>2022-02-04</v>
       </c>
       <c r="B824" t="str">
-        <v>Transportation</v>
+        <v>Food</v>
       </c>
       <c r="C824">
-        <v>950</v>
+        <v>30</v>
       </c>
       <c r="D824" t="str">
-        <v>Bike's New Battery</v>
+        <v>Water</v>
       </c>
     </row>
     <row r="825">
       <c r="A825" t="str">
-        <v>2022-02-04</v>
+        <v>2022-01-28</v>
       </c>
       <c r="B825" t="str">
-        <v>Food</v>
+        <v>Entertainment</v>
       </c>
       <c r="C825">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="D825" t="str">
-        <v>Water</v>
+        <v>Spotify</v>
       </c>
     </row>
     <row r="826">
       <c r="A826" t="str">
-        <v>2022-01-28</v>
+        <v>2022-02-04</v>
       </c>
       <c r="B826" t="str">
-        <v>Entertainment</v>
+        <v>Food</v>
       </c>
       <c r="C826">
-        <v>119</v>
+        <v>406</v>
       </c>
       <c r="D826" t="str">
-        <v>Spotify</v>
+        <v>Blinkit</v>
       </c>
     </row>
     <row r="827">
       <c r="A827" t="str">
-        <v>2022-02-04</v>
+        <v>2022-01-29</v>
       </c>
       <c r="B827" t="str">
-        <v>Food</v>
+        <v>Transportation</v>
       </c>
       <c r="C827">
-        <v>406</v>
+        <v>210</v>
       </c>
       <c r="D827" t="str">
-        <v>Blinkit</v>
+        <v>Petrol</v>
       </c>
     </row>
     <row r="828">
@@ -11867,52 +11867,52 @@
         <v>2022-01-29</v>
       </c>
       <c r="B828" t="str">
-        <v>Transportation</v>
+        <v>Other Income</v>
       </c>
       <c r="C828">
-        <v>210</v>
+        <v>809</v>
       </c>
       <c r="D828" t="str">
-        <v>Petrol</v>
+        <v>Amazon Cashback</v>
       </c>
     </row>
     <row r="829">
       <c r="A829" t="str">
-        <v>2022-01-29</v>
+        <v>2022-02-12</v>
       </c>
       <c r="B829" t="str">
-        <v>Other Income</v>
+        <v>Food</v>
       </c>
       <c r="C829">
-        <v>809</v>
+        <v>488</v>
       </c>
       <c r="D829" t="str">
-        <v>Amazon Cashback</v>
+        <v>Blinkit</v>
       </c>
     </row>
     <row r="830">
       <c r="A830" t="str">
-        <v>2022-02-12</v>
+        <v>2022-02-14</v>
       </c>
       <c r="B830" t="str">
         <v>Food</v>
       </c>
       <c r="C830">
-        <v>488</v>
+        <v>168</v>
       </c>
       <c r="D830" t="str">
-        <v>Blinkit</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="831">
       <c r="A831" t="str">
-        <v>2022-02-14</v>
+        <v>2022-02-15</v>
       </c>
       <c r="B831" t="str">
         <v>Food</v>
       </c>
       <c r="C831">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D831" t="str">
         <v>Swiggy</v>
@@ -11923,41 +11923,41 @@
         <v>2022-02-15</v>
       </c>
       <c r="B832" t="str">
-        <v>Food</v>
+        <v>Home</v>
       </c>
       <c r="C832">
-        <v>158</v>
+        <v>60</v>
       </c>
       <c r="D832" t="str">
-        <v>Swiggy</v>
+        <v>Garbage</v>
       </c>
     </row>
     <row r="833">
       <c r="A833" t="str">
-        <v>2022-02-15</v>
+        <v>2022-02-17</v>
       </c>
       <c r="B833" t="str">
-        <v>Home</v>
+        <v>Food</v>
       </c>
       <c r="C833">
-        <v>60</v>
+        <v>146</v>
       </c>
       <c r="D833" t="str">
-        <v>Garbage</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="834">
       <c r="A834" t="str">
-        <v>2022-02-17</v>
+        <v>2022-02-18</v>
       </c>
       <c r="B834" t="str">
-        <v>Food</v>
+        <v>Home</v>
       </c>
       <c r="C834">
-        <v>146</v>
+        <v>9000</v>
       </c>
       <c r="D834" t="str">
-        <v>Swiggy</v>
+        <v>Rent</v>
       </c>
     </row>
     <row r="835">
@@ -11965,13 +11965,13 @@
         <v>2022-02-18</v>
       </c>
       <c r="B835" t="str">
-        <v>Home</v>
+        <v>Food</v>
       </c>
       <c r="C835">
-        <v>9000</v>
+        <v>100</v>
       </c>
       <c r="D835" t="str">
-        <v>Rent</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="836">
@@ -11979,13 +11979,13 @@
         <v>2022-02-18</v>
       </c>
       <c r="B836" t="str">
-        <v>Food</v>
+        <v>Transportation</v>
       </c>
       <c r="C836">
-        <v>100</v>
+        <v>5760</v>
       </c>
       <c r="D836" t="str">
-        <v>Swiggy</v>
+        <v>Flight: Trip to Nepal</v>
       </c>
     </row>
     <row r="837">
@@ -11993,24 +11993,24 @@
         <v>2022-02-18</v>
       </c>
       <c r="B837" t="str">
-        <v>Transportation</v>
+        <v>Food</v>
       </c>
       <c r="C837">
-        <v>5760</v>
+        <v>104</v>
       </c>
       <c r="D837" t="str">
-        <v>Flight: Trip to Nepal</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="838">
       <c r="A838" t="str">
-        <v>2022-02-18</v>
+        <v>2022-02-19</v>
       </c>
       <c r="B838" t="str">
         <v>Food</v>
       </c>
       <c r="C838">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D838" t="str">
         <v>Swiggy</v>
@@ -12021,13 +12021,13 @@
         <v>2022-02-19</v>
       </c>
       <c r="B839" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C839">
-        <v>110</v>
+        <v>1846</v>
       </c>
       <c r="D839" t="str">
-        <v>Swiggy</v>
+        <v>Flipkart</v>
       </c>
     </row>
     <row r="840">
@@ -12038,10 +12038,10 @@
         <v>Shopping</v>
       </c>
       <c r="C840">
-        <v>1846</v>
+        <v>999</v>
       </c>
       <c r="D840" t="str">
-        <v>Flipkart</v>
+        <v xml:space="preserve">Myntra </v>
       </c>
     </row>
     <row r="841">
@@ -12049,24 +12049,24 @@
         <v>2022-02-19</v>
       </c>
       <c r="B841" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C841">
-        <v>999</v>
+        <v>118</v>
       </c>
       <c r="D841" t="str">
-        <v xml:space="preserve">Myntra </v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="842">
       <c r="A842" t="str">
-        <v>2022-02-19</v>
+        <v>2022-02-20</v>
       </c>
       <c r="B842" t="str">
         <v>Food</v>
       </c>
       <c r="C842">
-        <v>118</v>
+        <v>171</v>
       </c>
       <c r="D842" t="str">
         <v>Swiggy</v>
@@ -12080,10 +12080,10 @@
         <v>Food</v>
       </c>
       <c r="C843">
-        <v>171</v>
+        <v>574</v>
       </c>
       <c r="D843" t="str">
-        <v>Swiggy</v>
+        <v>Bigbasket</v>
       </c>
     </row>
     <row r="844">
@@ -12094,38 +12094,38 @@
         <v>Food</v>
       </c>
       <c r="C844">
-        <v>574</v>
+        <v>211</v>
       </c>
       <c r="D844" t="str">
-        <v>Bigbasket</v>
+        <v>Water and dairy</v>
       </c>
     </row>
     <row r="845">
       <c r="A845" t="str">
-        <v>2022-02-20</v>
+        <v>2022-02-22</v>
       </c>
       <c r="B845" t="str">
-        <v>Food</v>
+        <v>Transportation</v>
       </c>
       <c r="C845">
-        <v>211</v>
+        <v>5771</v>
       </c>
       <c r="D845" t="str">
-        <v>Water and dairy</v>
+        <v>Flight: Trip to India</v>
       </c>
     </row>
     <row r="846">
       <c r="A846" t="str">
-        <v>2022-02-22</v>
+        <v>2022-02-23</v>
       </c>
       <c r="B846" t="str">
-        <v>Transportation</v>
+        <v>Shopping</v>
       </c>
       <c r="C846">
-        <v>5771</v>
+        <v>369</v>
       </c>
       <c r="D846" t="str">
-        <v>Flight: Trip to India</v>
+        <v>Amazon</v>
       </c>
     </row>
     <row r="847">
@@ -12133,13 +12133,13 @@
         <v>2022-02-23</v>
       </c>
       <c r="B847" t="str">
-        <v>Shopping</v>
+        <v>Bills</v>
       </c>
       <c r="C847">
-        <v>369</v>
+        <v>589</v>
       </c>
       <c r="D847" t="str">
-        <v>Amazon</v>
+        <v>Airtel Wifi Mainpuri</v>
       </c>
     </row>
     <row r="848">
@@ -12147,41 +12147,41 @@
         <v>2022-02-23</v>
       </c>
       <c r="B848" t="str">
-        <v>Bills</v>
+        <v>HealthCare</v>
       </c>
       <c r="C848">
-        <v>589</v>
+        <v>500</v>
       </c>
       <c r="D848" t="str">
-        <v>Airtel Wifi Mainpuri</v>
+        <v>Covid 19 RT-PCR</v>
       </c>
     </row>
     <row r="849">
       <c r="A849" t="str">
-        <v>2022-02-23</v>
+        <v>2022-02-24</v>
       </c>
       <c r="B849" t="str">
-        <v>HealthCare</v>
+        <v>Shopping</v>
       </c>
       <c r="C849">
-        <v>500</v>
+        <v>130</v>
       </c>
       <c r="D849" t="str">
-        <v>Covid 19 RT-PCR</v>
+        <v>Amazon</v>
       </c>
     </row>
     <row r="850">
       <c r="A850" t="str">
-        <v>2022-02-24</v>
+        <v>2022-02-25</v>
       </c>
       <c r="B850" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C850">
-        <v>130</v>
+        <v>854</v>
       </c>
       <c r="D850" t="str">
-        <v>Amazon</v>
+        <v>Bigbasket</v>
       </c>
     </row>
     <row r="851">
@@ -12189,27 +12189,27 @@
         <v>2022-02-25</v>
       </c>
       <c r="B851" t="str">
-        <v>Food</v>
+        <v>Education</v>
       </c>
       <c r="C851">
-        <v>854</v>
+        <v>60</v>
       </c>
       <c r="D851" t="str">
-        <v>Bigbasket</v>
+        <v>Printouts</v>
       </c>
     </row>
     <row r="852">
       <c r="A852" t="str">
-        <v>2022-02-25</v>
+        <v>2022-02-26</v>
       </c>
       <c r="B852" t="str">
-        <v>Education</v>
+        <v>Transportation</v>
       </c>
       <c r="C852">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D852" t="str">
-        <v>Printouts</v>
+        <v>Uber</v>
       </c>
     </row>
     <row r="853">
@@ -12217,41 +12217,41 @@
         <v>2022-02-26</v>
       </c>
       <c r="B853" t="str">
-        <v>Transportation</v>
+        <v>Bills</v>
       </c>
       <c r="C853">
-        <v>150</v>
+        <v>755</v>
       </c>
       <c r="D853" t="str">
-        <v>Uber</v>
+        <v xml:space="preserve">Airtel international roaming </v>
       </c>
     </row>
     <row r="854">
       <c r="A854" t="str">
-        <v>2022-02-26</v>
+        <v>2022-02-27</v>
       </c>
       <c r="B854" t="str">
-        <v>Bills</v>
+        <v>Vacation</v>
       </c>
       <c r="C854">
-        <v>755</v>
+        <v>21562</v>
       </c>
       <c r="D854" t="str">
-        <v xml:space="preserve">Airtel international roaming </v>
+        <v>Nepal Trip (Chhen Bed &amp; Breakfast Hotel and Cab)</v>
       </c>
     </row>
     <row r="855">
       <c r="A855" t="str">
-        <v>2022-02-27</v>
+        <v>2022-02-28</v>
       </c>
       <c r="B855" t="str">
-        <v>Vacation</v>
+        <v>Bills</v>
       </c>
       <c r="C855">
-        <v>21562</v>
+        <v>589</v>
       </c>
       <c r="D855" t="str">
-        <v>Nepal Trip (Chhen Bed &amp; Breakfast Hotel and Cab)</v>
+        <v>Airtel Wifi Delhi</v>
       </c>
     </row>
     <row r="856">
@@ -12259,55 +12259,55 @@
         <v>2022-02-28</v>
       </c>
       <c r="B856" t="str">
-        <v>Bills</v>
+        <v>Entertainment</v>
       </c>
       <c r="C856">
-        <v>589</v>
+        <v>119</v>
       </c>
       <c r="D856" t="str">
-        <v>Airtel Wifi Delhi</v>
+        <v>Spotify</v>
       </c>
     </row>
     <row r="857">
       <c r="A857" t="str">
-        <v>2022-02-28</v>
+        <v>2022-03-01</v>
       </c>
       <c r="B857" t="str">
         <v>Entertainment</v>
       </c>
       <c r="C857">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="D857" t="str">
-        <v>Spotify</v>
+        <v>Youtube</v>
       </c>
     </row>
     <row r="858">
       <c r="A858" t="str">
-        <v>2022-03-01</v>
+        <v>2022-02-28</v>
       </c>
       <c r="B858" t="str">
-        <v>Entertainment</v>
+        <v>Other Income</v>
       </c>
       <c r="C858">
-        <v>129</v>
+        <v>627</v>
       </c>
       <c r="D858" t="str">
-        <v>Youtube</v>
+        <v>Amazon Cashback</v>
       </c>
     </row>
     <row r="859">
       <c r="A859" t="str">
-        <v>2022-02-28</v>
+        <v>2022-03-05</v>
       </c>
       <c r="B859" t="str">
-        <v>Other Income</v>
+        <v>Food</v>
       </c>
       <c r="C859">
-        <v>627</v>
+        <v>899</v>
       </c>
       <c r="D859" t="str">
-        <v>Amazon Cashback</v>
+        <v>Swiggy One</v>
       </c>
     </row>
     <row r="860">
@@ -12318,10 +12318,10 @@
         <v>Food</v>
       </c>
       <c r="C860">
-        <v>899</v>
+        <v>158</v>
       </c>
       <c r="D860" t="str">
-        <v>Swiggy One</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="861">
@@ -12329,13 +12329,13 @@
         <v>2022-03-05</v>
       </c>
       <c r="B861" t="str">
-        <v>Food</v>
+        <v>Transportation</v>
       </c>
       <c r="C861">
-        <v>158</v>
+        <v>40</v>
       </c>
       <c r="D861" t="str">
-        <v>Swiggy</v>
+        <v>Rickshaw</v>
       </c>
     </row>
     <row r="862">
@@ -12343,41 +12343,41 @@
         <v>2022-03-05</v>
       </c>
       <c r="B862" t="str">
-        <v>Transportation</v>
+        <v>Food</v>
       </c>
       <c r="C862">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="D862" t="str">
-        <v>Rickshaw</v>
+        <v>Water and dairy</v>
       </c>
     </row>
     <row r="863">
       <c r="A863" t="str">
-        <v>2022-03-05</v>
+        <v>2022-03-07</v>
       </c>
       <c r="B863" t="str">
-        <v>Food</v>
+        <v>Salary</v>
       </c>
       <c r="C863">
-        <v>146</v>
+        <v>81120</v>
       </c>
       <c r="D863" t="str">
-        <v>Water and dairy</v>
+        <v/>
       </c>
     </row>
     <row r="864">
       <c r="A864" t="str">
-        <v>2022-03-07</v>
+        <v>2022-03-06</v>
       </c>
       <c r="B864" t="str">
-        <v>Salary</v>
+        <v>Grocery</v>
       </c>
       <c r="C864">
-        <v>81120</v>
+        <v>610</v>
       </c>
       <c r="D864" t="str">
-        <v/>
+        <v>Blinkit</v>
       </c>
     </row>
     <row r="865">
@@ -12388,10 +12388,10 @@
         <v>Grocery</v>
       </c>
       <c r="C865">
-        <v>610</v>
+        <v>1156</v>
       </c>
       <c r="D865" t="str">
-        <v>Blinkit</v>
+        <v>Bigbasket</v>
       </c>
     </row>
     <row r="866">
@@ -12399,69 +12399,69 @@
         <v>2022-03-06</v>
       </c>
       <c r="B866" t="str">
-        <v>Grocery</v>
+        <v>Bills</v>
       </c>
       <c r="C866">
-        <v>1156</v>
+        <v>75</v>
       </c>
       <c r="D866" t="str">
-        <v>Bigbasket</v>
+        <v>iCloud</v>
       </c>
     </row>
     <row r="867">
       <c r="A867" t="str">
-        <v>2022-03-06</v>
+        <v>2022-03-08</v>
       </c>
       <c r="B867" t="str">
-        <v>Bills</v>
+        <v>Food</v>
       </c>
       <c r="C867">
-        <v>75</v>
+        <v>173</v>
       </c>
       <c r="D867" t="str">
-        <v>iCloud</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="868">
       <c r="A868" t="str">
-        <v>2022-03-08</v>
+        <v>2022-02-27</v>
       </c>
       <c r="B868" t="str">
-        <v>Food</v>
+        <v>Vacation</v>
       </c>
       <c r="C868">
-        <v>173</v>
+        <v>15000</v>
       </c>
       <c r="D868" t="str">
-        <v>Swiggy</v>
+        <v>Nepal Trip (Food, Meridian Hotel and Cab)</v>
       </c>
     </row>
     <row r="869">
       <c r="A869" t="str">
-        <v>2022-02-27</v>
+        <v>2022-03-05</v>
       </c>
       <c r="B869" t="str">
         <v>Vacation</v>
       </c>
       <c r="C869">
-        <v>15000</v>
+        <v>3195</v>
       </c>
       <c r="D869" t="str">
-        <v>Nepal Trip (Food, Meridian Hotel and Cab)</v>
+        <v>To Abineesha (Nepal Trip)</v>
       </c>
     </row>
     <row r="870">
       <c r="A870" t="str">
-        <v>2022-03-05</v>
+        <v>2022-03-08</v>
       </c>
       <c r="B870" t="str">
-        <v>Vacation</v>
+        <v>Home</v>
       </c>
       <c r="C870">
-        <v>3195</v>
+        <v>200</v>
       </c>
       <c r="D870" t="str">
-        <v>To Abineesha (Nepal Trip)</v>
+        <v xml:space="preserve">Maintenance </v>
       </c>
     </row>
     <row r="871">
@@ -12469,52 +12469,52 @@
         <v>2022-03-08</v>
       </c>
       <c r="B871" t="str">
-        <v>Home</v>
+        <v>Food</v>
       </c>
       <c r="C871">
-        <v>200</v>
+        <v>158</v>
       </c>
       <c r="D871" t="str">
-        <v xml:space="preserve">Maintenance </v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="872">
       <c r="A872" t="str">
-        <v>2022-03-08</v>
+        <v>2022-03-09</v>
       </c>
       <c r="B872" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C872">
-        <v>158</v>
+        <v>1593</v>
       </c>
       <c r="D872" t="str">
-        <v>Swiggy</v>
+        <v>Myntra</v>
       </c>
     </row>
     <row r="873">
       <c r="A873" t="str">
-        <v>2022-03-09</v>
+        <v>2022-03-10</v>
       </c>
       <c r="B873" t="str">
         <v>Shopping</v>
       </c>
       <c r="C873">
-        <v>1593</v>
+        <v>1783</v>
       </c>
       <c r="D873" t="str">
-        <v>Myntra</v>
+        <v>Amazon</v>
       </c>
     </row>
     <row r="874">
       <c r="A874" t="str">
-        <v>2022-03-10</v>
+        <v>2022-03-11</v>
       </c>
       <c r="B874" t="str">
         <v>Shopping</v>
       </c>
       <c r="C874">
-        <v>1783</v>
+        <v>245</v>
       </c>
       <c r="D874" t="str">
         <v>Amazon</v>
@@ -12525,13 +12525,13 @@
         <v>2022-03-11</v>
       </c>
       <c r="B875" t="str">
-        <v>Shopping</v>
+        <v>Grocery</v>
       </c>
       <c r="C875">
-        <v>245</v>
+        <v>477</v>
       </c>
       <c r="D875" t="str">
-        <v>Amazon</v>
+        <v>Blinkit</v>
       </c>
     </row>
     <row r="876">
@@ -12539,27 +12539,27 @@
         <v>2022-03-11</v>
       </c>
       <c r="B876" t="str">
-        <v>Grocery</v>
+        <v>Shopping</v>
       </c>
       <c r="C876">
-        <v>477</v>
+        <v>751</v>
       </c>
       <c r="D876" t="str">
-        <v>Blinkit</v>
+        <v>Bulbs Syska flipkart</v>
       </c>
     </row>
     <row r="877">
       <c r="A877" t="str">
-        <v>2022-03-11</v>
+        <v>2022-03-12</v>
       </c>
       <c r="B877" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C877">
-        <v>751</v>
+        <v>187</v>
       </c>
       <c r="D877" t="str">
-        <v>Bulbs Syska flipkart</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="878">
@@ -12567,41 +12567,41 @@
         <v>2022-03-12</v>
       </c>
       <c r="B878" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C878">
-        <v>187</v>
+        <v>1749</v>
       </c>
       <c r="D878" t="str">
-        <v>Swiggy</v>
+        <v>Flipkart Wireless bell</v>
       </c>
     </row>
     <row r="879">
       <c r="A879" t="str">
-        <v>2022-03-12</v>
+        <v>2022-03-13</v>
       </c>
       <c r="B879" t="str">
-        <v>Shopping</v>
+        <v>Grocery</v>
       </c>
       <c r="C879">
-        <v>1749</v>
+        <v>586</v>
       </c>
       <c r="D879" t="str">
-        <v>Flipkart Wireless bell</v>
+        <v>Blinkit</v>
       </c>
     </row>
     <row r="880">
       <c r="A880" t="str">
-        <v>2022-03-13</v>
+        <v>2022-03-14</v>
       </c>
       <c r="B880" t="str">
-        <v>Grocery</v>
+        <v>Transportation</v>
       </c>
       <c r="C880">
-        <v>586</v>
+        <v>1089</v>
       </c>
       <c r="D880" t="str">
-        <v>Blinkit</v>
+        <v>IRCTC Trip to Mainpuri</v>
       </c>
     </row>
     <row r="881">
@@ -12612,52 +12612,52 @@
         <v>Transportation</v>
       </c>
       <c r="C881">
-        <v>1089</v>
+        <v>100</v>
       </c>
       <c r="D881" t="str">
-        <v>IRCTC Trip to Mainpuri</v>
+        <v xml:space="preserve">Metro card recharge </v>
       </c>
     </row>
     <row r="882">
       <c r="A882" t="str">
-        <v>2022-03-14</v>
+        <v>2022-03-17</v>
       </c>
       <c r="B882" t="str">
-        <v>Transportation</v>
+        <v>Home</v>
       </c>
       <c r="C882">
-        <v>100</v>
+        <v>9000</v>
       </c>
       <c r="D882" t="str">
-        <v xml:space="preserve">Metro card recharge </v>
+        <v>Rent</v>
       </c>
     </row>
     <row r="883">
       <c r="A883" t="str">
-        <v>2022-03-17</v>
+        <v>2022-03-18</v>
       </c>
       <c r="B883" t="str">
-        <v>Home</v>
+        <v>Shopping</v>
       </c>
       <c r="C883">
-        <v>9000</v>
+        <v>1600</v>
       </c>
       <c r="D883" t="str">
-        <v>Rent</v>
+        <v>Amazon Shoes for papa</v>
       </c>
     </row>
     <row r="884">
       <c r="A884" t="str">
-        <v>2022-03-18</v>
+        <v>2022-03-22</v>
       </c>
       <c r="B884" t="str">
-        <v>Shopping</v>
+        <v>Cashback</v>
       </c>
       <c r="C884">
-        <v>1600</v>
+        <v>585</v>
       </c>
       <c r="D884" t="str">
-        <v>Amazon Shoes for papa</v>
+        <v>Flipkart Cashback</v>
       </c>
     </row>
     <row r="885">
@@ -12665,27 +12665,27 @@
         <v>2022-03-22</v>
       </c>
       <c r="B885" t="str">
-        <v>Cashback</v>
+        <v>Shopping</v>
       </c>
       <c r="C885">
-        <v>585</v>
+        <v>676</v>
       </c>
       <c r="D885" t="str">
-        <v>Flipkart Cashback</v>
+        <v>Amazon</v>
       </c>
     </row>
     <row r="886">
       <c r="A886" t="str">
-        <v>2022-03-22</v>
+        <v>2022-03-23</v>
       </c>
       <c r="B886" t="str">
         <v>Shopping</v>
       </c>
       <c r="C886">
-        <v>676</v>
+        <v>200</v>
       </c>
       <c r="D886" t="str">
-        <v>Amazon</v>
+        <v>Amazon bulb</v>
       </c>
     </row>
     <row r="887">
@@ -12693,13 +12693,13 @@
         <v>2022-03-23</v>
       </c>
       <c r="B887" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C887">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="D887" t="str">
-        <v>Amazon bulb</v>
+        <v>Water</v>
       </c>
     </row>
     <row r="888">
@@ -12710,10 +12710,10 @@
         <v>Food</v>
       </c>
       <c r="C888">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="D888" t="str">
-        <v>Water</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="889">
@@ -12721,27 +12721,27 @@
         <v>2022-03-23</v>
       </c>
       <c r="B889" t="str">
-        <v>Food</v>
+        <v>Shopping</v>
       </c>
       <c r="C889">
-        <v>133</v>
+        <v>2675</v>
       </c>
       <c r="D889" t="str">
-        <v>Swiggy</v>
+        <v>Laptop 8GB RAM</v>
       </c>
     </row>
     <row r="890">
       <c r="A890" t="str">
-        <v>2022-03-23</v>
+        <v>2022-03-24</v>
       </c>
       <c r="B890" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C890">
-        <v>2675</v>
+        <v>128</v>
       </c>
       <c r="D890" t="str">
-        <v>Laptop 8GB RAM</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="891">
@@ -12749,10 +12749,10 @@
         <v>2022-03-24</v>
       </c>
       <c r="B891" t="str">
-        <v>Food</v>
+        <v>Grocery</v>
       </c>
       <c r="C891">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D891" t="str">
         <v>Swiggy</v>
@@ -12763,13 +12763,13 @@
         <v>2022-03-24</v>
       </c>
       <c r="B892" t="str">
-        <v>Grocery</v>
+        <v>Transportation</v>
       </c>
       <c r="C892">
-        <v>123</v>
+        <v>5172</v>
       </c>
       <c r="D892" t="str">
-        <v>Swiggy</v>
+        <v>Flight to Nepal</v>
       </c>
     </row>
     <row r="893">
@@ -12777,27 +12777,27 @@
         <v>2022-03-24</v>
       </c>
       <c r="B893" t="str">
-        <v>Vacation</v>
+        <v>Shopping</v>
       </c>
       <c r="C893">
-        <v>5172</v>
+        <v>399</v>
       </c>
       <c r="D893" t="str">
-        <v>Flight to Nepal</v>
+        <v>Bedsheet from Flipkart</v>
       </c>
     </row>
     <row r="894">
       <c r="A894" t="str">
-        <v>2022-03-24</v>
+        <v>2022-03-25</v>
       </c>
       <c r="B894" t="str">
         <v>Shopping</v>
       </c>
       <c r="C894">
-        <v>399</v>
+        <v>2777</v>
       </c>
       <c r="D894" t="str">
-        <v>Bedsheet from Flipkart</v>
+        <v>Amazon (Induction + Kadhai)</v>
       </c>
     </row>
     <row r="895">
@@ -12808,10 +12808,10 @@
         <v>Shopping</v>
       </c>
       <c r="C895">
-        <v>2777</v>
+        <v>1580</v>
       </c>
       <c r="D895" t="str">
-        <v>Amazon (Induction + Kadhai)</v>
+        <v>Flipkart Hawkins cooker</v>
       </c>
     </row>
     <row r="896">
@@ -12819,27 +12819,27 @@
         <v>2022-03-25</v>
       </c>
       <c r="B896" t="str">
-        <v>Shopping</v>
+        <v>Food</v>
       </c>
       <c r="C896">
-        <v>1580</v>
+        <v>142</v>
       </c>
       <c r="D896" t="str">
-        <v>Flipkart Hawkins cooker</v>
+        <v>Swiggy</v>
       </c>
     </row>
     <row r="897">
       <c r="A897" t="str">
-        <v>2022-03-25</v>
+        <v>2022-03-26</v>
       </c>
       <c r="B897" t="str">
-        <v>Food</v>
+        <v>Bills</v>
       </c>
       <c r="C897">
-        <v>142</v>
+        <v>3004</v>
       </c>
       <c r="D897" t="str">
-        <v>Swiggy</v>
+        <v>Airtel Wifi Mainpuri 6 months</v>
       </c>
     </row>
     <row r="898">
@@ -12847,46 +12847,1138 @@
         <v>2022-03-26</v>
       </c>
       <c r="B898" t="str">
-        <v>Shopping</v>
+        <v>Grocery</v>
       </c>
       <c r="C898">
-        <v>199</v>
+        <v>588</v>
       </c>
       <c r="D898" t="str">
-        <v>Induction base pan</v>
+        <v>Blinkit</v>
       </c>
     </row>
     <row r="899">
       <c r="A899" t="str">
-        <v>2022-03-26</v>
+        <v>2022-03-28</v>
       </c>
       <c r="B899" t="str">
         <v>Bills</v>
       </c>
       <c r="C899">
-        <v>3004</v>
+        <v>589</v>
       </c>
       <c r="D899" t="str">
-        <v>Airtel Wifi Mainpuri 6 months</v>
+        <v>Airtel wifi Delhi</v>
       </c>
     </row>
     <row r="900">
       <c r="A900" t="str">
-        <v>2022-03-26</v>
+        <v>2022-03-28</v>
       </c>
       <c r="B900" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C900">
+        <v>119</v>
+      </c>
+      <c r="D900" t="str">
+        <v>Spotify</v>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="str">
+        <v>2022-03-28</v>
+      </c>
+      <c r="B901" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C901">
+        <v>179</v>
+      </c>
+      <c r="D901" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="str">
+        <v>2022-03-29</v>
+      </c>
+      <c r="B902" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C902">
+        <v>1624</v>
+      </c>
+      <c r="D902" t="str">
+        <v xml:space="preserve">Flipkart Abineesha's clothes </v>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="str">
+        <v>2022-03-29</v>
+      </c>
+      <c r="B903" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C903">
+        <v>158</v>
+      </c>
+      <c r="D903" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="str">
+        <v>2022-03-29</v>
+      </c>
+      <c r="B904" t="str">
+        <v>Cashback</v>
+      </c>
+      <c r="C904">
+        <v>450</v>
+      </c>
+      <c r="D904" t="str">
+        <v>Amazon Cashback</v>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="str">
+        <v>2022-03-30</v>
+      </c>
+      <c r="B905" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C905">
+        <v>321</v>
+      </c>
+      <c r="D905" t="str">
+        <v>Amazon</v>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="str">
+        <v>2022-03-30</v>
+      </c>
+      <c r="B906" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C906">
+        <v>121</v>
+      </c>
+      <c r="D906" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="str">
+        <v>2022-03-30</v>
+      </c>
+      <c r="B907" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C907">
+        <v>123</v>
+      </c>
+      <c r="D907" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="str">
+        <v>2022-04-01</v>
+      </c>
+      <c r="B908" t="str">
+        <v>Vacation</v>
+      </c>
+      <c r="C908">
+        <v>38000</v>
+      </c>
+      <c r="D908" t="str">
+        <v>Nepal Trip: Stay with Abineesha + Expenses April/May</v>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="str">
+        <v>2022-03-31</v>
+      </c>
+      <c r="B909" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C909">
+        <v>122</v>
+      </c>
+      <c r="D909" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="str">
+        <v>2022-03-31</v>
+      </c>
+      <c r="B910" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C910">
+        <v>158</v>
+      </c>
+      <c r="D910" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="str">
+        <v>2022-04-01</v>
+      </c>
+      <c r="B911" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C911">
+        <v>129</v>
+      </c>
+      <c r="D911" t="str">
+        <v xml:space="preserve">Youtube premium </v>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="str">
+        <v>2022-03-31</v>
+      </c>
+      <c r="B912" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C912">
+        <v>1225</v>
+      </c>
+      <c r="D912" t="str">
+        <v>Refund shopping Abineesha's clothes</v>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="str">
+        <v>2022-04-03</v>
+      </c>
+      <c r="B913" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C913">
+        <v>799</v>
+      </c>
+      <c r="D913" t="str">
+        <v>Airtel International roaming</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="str">
+        <v>2022-04-03</v>
+      </c>
+      <c r="B914" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C914">
+        <v>120</v>
+      </c>
+      <c r="D914" t="str">
+        <v>Uber</v>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="str">
+        <v>2022-04-07</v>
+      </c>
+      <c r="B915" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C915">
+        <v>81120</v>
+      </c>
+      <c r="D915" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="str">
+        <v>2022-04-17</v>
+      </c>
+      <c r="B916" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C916">
+        <v>9000</v>
+      </c>
+      <c r="D916" t="str">
+        <v>Rent</v>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="str">
+        <v>2022-04-23</v>
+      </c>
+      <c r="B917" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C917">
+        <v>429</v>
+      </c>
+      <c r="D917" t="str">
+        <v>Airtel wifi delhi</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="str">
+        <v>2022-05-01</v>
+      </c>
+      <c r="B918" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C918">
+        <v>6105</v>
+      </c>
+      <c r="D918" t="str">
+        <v>Flight to India</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="str">
+        <v>2022-05-01</v>
+      </c>
+      <c r="B919" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C919">
+        <v>129</v>
+      </c>
+      <c r="D919" t="str">
+        <v>Youtube</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="str">
+        <v>2022-05-01</v>
+      </c>
+      <c r="B920" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C920">
+        <v>1929</v>
+      </c>
+      <c r="D920" t="str">
+        <v>Flight to India - Reschedule</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="str">
+        <v>2022-05-06</v>
+      </c>
+      <c r="B921" t="str">
+        <v>Vacation</v>
+      </c>
+      <c r="C921">
+        <v>12500</v>
+      </c>
+      <c r="D921" t="str">
+        <v>To Abineesha (Pokhra Trip)</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="str">
+        <v>2022-05-06</v>
+      </c>
+      <c r="B922" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C922">
+        <v>86783</v>
+      </c>
+      <c r="D922" t="str">
+        <v>Salary for the month April</v>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="str">
+        <v>2022-05-17</v>
+      </c>
+      <c r="B923" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C923">
+        <v>9000</v>
+      </c>
+      <c r="D923" t="str">
+        <v>Rent</v>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="str">
+        <v>2022-05-17</v>
+      </c>
+      <c r="B924" t="str">
+        <v>Vacation</v>
+      </c>
+      <c r="C924">
+        <v>6265</v>
+      </c>
+      <c r="D924" t="str">
+        <v>To Abineesha(Expenses)</v>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="str">
+        <v>2022-05-17</v>
+      </c>
+      <c r="B925" t="str">
+        <v>Cashback</v>
+      </c>
+      <c r="C925">
+        <v>528</v>
+      </c>
+      <c r="D925" t="str">
+        <v>MMT Delhi to Chennai flight</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="str">
+        <v>2022-05-23</v>
+      </c>
+      <c r="B926" t="str">
+        <v>Vacation</v>
+      </c>
+      <c r="C926">
+        <v>5000</v>
+      </c>
+      <c r="D926" t="str">
+        <v>Hotel Krishna Kathmandu</v>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="str">
+        <v>2022-05-24</v>
+      </c>
+      <c r="B927" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C927">
+        <v>236</v>
+      </c>
+      <c r="D927" t="str">
+        <v>Airtel Wifi Delhi</v>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="str">
+        <v>2022-05-24</v>
+      </c>
+      <c r="B928" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C928">
+        <v>168</v>
+      </c>
+      <c r="D928" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="str">
+        <v>2022-05-25</v>
+      </c>
+      <c r="B929" t="str">
         <v>Grocery</v>
       </c>
-      <c r="C900">
-        <v>588</v>
-      </c>
-      <c r="D900" t="str">
+      <c r="C929">
+        <v>918</v>
+      </c>
+      <c r="D929" t="str">
         <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="str">
+        <v>2022-05-25</v>
+      </c>
+      <c r="B930" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C930">
+        <v>131</v>
+      </c>
+      <c r="D930" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="str">
+        <v>2022-05-27</v>
+      </c>
+      <c r="B931" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C931">
+        <v>603</v>
+      </c>
+      <c r="D931" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="str">
+        <v>2022-05-28</v>
+      </c>
+      <c r="B932" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C932">
+        <v>119</v>
+      </c>
+      <c r="D932" t="str">
+        <v>Spotify</v>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="str">
+        <v>2022-05-28</v>
+      </c>
+      <c r="B933" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C933">
+        <v>146</v>
+      </c>
+      <c r="D933" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="str">
+        <v>2022-05-30</v>
+      </c>
+      <c r="B934" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C934">
+        <v>116</v>
+      </c>
+      <c r="D934" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="str">
+        <v>2022-06-01</v>
+      </c>
+      <c r="B935" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C935">
+        <v>1085</v>
+      </c>
+      <c r="D935" t="str">
+        <v>Bigbasket</v>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="str">
+        <v>2022-06-01</v>
+      </c>
+      <c r="B936" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C936">
+        <v>628</v>
+      </c>
+      <c r="D936" t="str">
+        <v>Amazon</v>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="str">
+        <v>2022-06-01</v>
+      </c>
+      <c r="B937" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C937">
+        <v>90</v>
+      </c>
+      <c r="D937" t="str">
+        <v>Water and Dairy</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="str">
+        <v>2022-06-01</v>
+      </c>
+      <c r="B938" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C938">
+        <v>129</v>
+      </c>
+      <c r="D938" t="str">
+        <v>Youtube</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="str">
+        <v>2022-06-05</v>
+      </c>
+      <c r="B939" t="str">
+        <v>Repairs</v>
+      </c>
+      <c r="C939">
+        <v>1200</v>
+      </c>
+      <c r="D939" t="str">
+        <v>Bike Service Credr Annual Subscription (4 times)</v>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="str">
+        <v>2022-06-06</v>
+      </c>
+      <c r="B940" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C940">
+        <v>1160</v>
+      </c>
+      <c r="D940" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="str">
+        <v>2022-06-05</v>
+      </c>
+      <c r="B941" t="str">
+        <v>Repairs</v>
+      </c>
+      <c r="C941">
+        <v>50</v>
+      </c>
+      <c r="D941" t="str">
+        <v xml:space="preserve">Bike meter check </v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="str">
+        <v>2022-06-06</v>
+      </c>
+      <c r="B942" t="str">
+        <v>Repairs</v>
+      </c>
+      <c r="C942">
+        <v>1400</v>
+      </c>
+      <c r="D942" t="str">
+        <v>Bike new digital meter pcb</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="str">
+        <v>2022-06-06</v>
+      </c>
+      <c r="B943" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C943">
+        <v>630</v>
+      </c>
+      <c r="D943" t="str">
+        <v>Petrol</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="str">
+        <v>2022-06-07</v>
+      </c>
+      <c r="B944" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C944">
+        <v>86783</v>
+      </c>
+      <c r="D944" t="str">
+        <v>Salary for the month May</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="str">
+        <v>2022-06-06</v>
+      </c>
+      <c r="B945" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C945">
+        <v>198</v>
+      </c>
+      <c r="D945" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="str">
+        <v>2022-06-07</v>
+      </c>
+      <c r="B946" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C946">
+        <v>126</v>
+      </c>
+      <c r="D946" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="str">
+        <v>2022-06-08</v>
+      </c>
+      <c r="B947" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C947">
+        <v>800</v>
+      </c>
+      <c r="D947" t="str">
+        <v>DDA Maintenance for Mar, Apr, May, June</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="str">
+        <v>2022-06-08</v>
+      </c>
+      <c r="B948" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C948">
+        <v>173</v>
+      </c>
+      <c r="D948" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="str">
+        <v>2022-06-09</v>
+      </c>
+      <c r="B949" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C949">
+        <v>84</v>
+      </c>
+      <c r="D949" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="str">
+        <v>2022-06-10</v>
+      </c>
+      <c r="B950" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C950">
+        <v>140</v>
+      </c>
+      <c r="D950" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="str">
+        <v>2022-06-11</v>
+      </c>
+      <c r="B951" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C951">
+        <v>704</v>
+      </c>
+      <c r="D951" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="str">
+        <v>2022-06-11</v>
+      </c>
+      <c r="B952" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C952">
+        <v>60</v>
+      </c>
+      <c r="D952" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="str">
+        <v>2022-06-12</v>
+      </c>
+      <c r="B953" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C953">
+        <v>144</v>
+      </c>
+      <c r="D953" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="str">
+        <v>2022-06-12</v>
+      </c>
+      <c r="B954" t="str">
+        <v>Repairs</v>
+      </c>
+      <c r="C954">
+        <v>238</v>
+      </c>
+      <c r="D954" t="str">
+        <v>UrbanClap Cooler Repair</v>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="str">
+        <v>2022-06-12</v>
+      </c>
+      <c r="B955" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C955">
+        <v>162</v>
+      </c>
+      <c r="D955" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="str">
+        <v>2022-06-12</v>
+      </c>
+      <c r="B956" t="str">
+        <v>Repairs</v>
+      </c>
+      <c r="C956">
+        <v>80</v>
+      </c>
+      <c r="D956" t="str">
+        <v>Bike wash and polish</v>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="str">
+        <v>2022-06-13</v>
+      </c>
+      <c r="B957" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C957">
+        <v>264</v>
+      </c>
+      <c r="D957" t="str">
+        <v>NACH: SBI</v>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="str">
+        <v>2022-05-11</v>
+      </c>
+      <c r="B958" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C958">
+        <v>144</v>
+      </c>
+      <c r="D958" t="str">
+        <v>NACH: HCL</v>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="str">
+        <v>2022-04-19</v>
+      </c>
+      <c r="B959" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C959">
+        <v>925</v>
+      </c>
+      <c r="D959" t="str">
+        <v>NACH: WIPRO</v>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="str">
+        <v>2022-03-24</v>
+      </c>
+      <c r="B960" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C960">
+        <v>316</v>
+      </c>
+      <c r="D960" t="str">
+        <v>SBI Interest</v>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="str">
+        <v>2022-03-05</v>
+      </c>
+      <c r="B961" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C961">
+        <v>43</v>
+      </c>
+      <c r="D961" t="str">
+        <v>NACH: CAM</v>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="str">
+        <v>2022-03-04</v>
+      </c>
+      <c r="B962" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C962">
+        <v>56</v>
+      </c>
+      <c r="D962" t="str">
+        <v>NACH: IRCTC</v>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="str">
+        <v>2022-03-03</v>
+      </c>
+      <c r="B963" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C963">
+        <v>24</v>
+      </c>
+      <c r="D963" t="str">
+        <v>NACH: Metropolis</v>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="str">
+        <v>2022-02-07</v>
+      </c>
+      <c r="B964" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C964">
+        <v>28</v>
+      </c>
+      <c r="D964" t="str">
+        <v>NACH: TCS</v>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="str">
+        <v>2022-02-04</v>
+      </c>
+      <c r="B965" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C965">
+        <v>60</v>
+      </c>
+      <c r="D965" t="str">
+        <v>NACH: HCL</v>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="str">
+        <v>2022-02-04</v>
+      </c>
+      <c r="B966" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C966">
+        <v>154</v>
+      </c>
+      <c r="D966" t="str">
+        <v>NACH: WIPRO</v>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="str">
+        <v>2021-12-25</v>
+      </c>
+      <c r="B967" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C967">
+        <v>276</v>
+      </c>
+      <c r="D967" t="str">
+        <v>SBI Credit Interest</v>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="str">
+        <v>2021-11-23</v>
+      </c>
+      <c r="B968" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C968">
+        <v>265</v>
+      </c>
+      <c r="D968" t="str">
+        <v>NACH: IOCL</v>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="str">
+        <v>2022-04-03</v>
+      </c>
+      <c r="B969" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C969">
+        <v>1727</v>
+      </c>
+      <c r="D969" t="str">
+        <v>UBI Credit Interest</v>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="str">
+        <v>2022-01-02</v>
+      </c>
+      <c r="B970" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C970">
+        <v>1375</v>
+      </c>
+      <c r="D970" t="str">
+        <v>UBI Credit Interest</v>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="str">
+        <v>2021-10-03</v>
+      </c>
+      <c r="B971" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C971">
+        <v>1892</v>
+      </c>
+      <c r="D971" t="str">
+        <v>UBI Credit Interest</v>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="str">
+        <v>2021-07-03</v>
+      </c>
+      <c r="B972" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C972">
+        <v>619</v>
+      </c>
+      <c r="D972" t="str">
+        <v>UBI Credit Interest</v>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="str">
+        <v>2020-10-04</v>
+      </c>
+      <c r="B973" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C973">
+        <v>834</v>
+      </c>
+      <c r="D973" t="str">
+        <v>UBI Credit</v>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="str">
+        <v>2022-06-14</v>
+      </c>
+      <c r="B974" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C974">
+        <v>175</v>
+      </c>
+      <c r="D974" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="str">
+        <v>2022-06-15</v>
+      </c>
+      <c r="B975" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C975">
+        <v>88</v>
+      </c>
+      <c r="D975" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="str">
+        <v>2022-06-15</v>
+      </c>
+      <c r="B976" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C976">
+        <v>116</v>
+      </c>
+      <c r="D976" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="str">
+        <v>2022-06-16</v>
+      </c>
+      <c r="B977" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C977">
+        <v>138</v>
+      </c>
+      <c r="D977" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="str">
+        <v>2022-06-16</v>
+      </c>
+      <c r="B978" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C978">
+        <v>9974.2</v>
+      </c>
+      <c r="D978" t="str">
+        <v>Airtel Wifi Delhi Annual Plan 100 mbps</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D900"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D978"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Expense distribution chart changed from column to bar
</commit_message>
<xml_diff>
--- a/spreadsheets/BudgetManager.xlsx
+++ b/spreadsheets/BudgetManager.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1050"/>
+  <dimension ref="A1:D1326"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4263,7 +4263,7 @@
         <v>2020-11-20</v>
       </c>
       <c r="B281" t="str">
-        <v>Bills</v>
+        <v>Other Income</v>
       </c>
       <c r="C281">
         <v>57</v>
@@ -4283,7 +4283,7 @@
         <v>1500</v>
       </c>
       <c r="D282" t="str">
-        <v>Amazon Gift Card - Diwali Gift</v>
+        <v>Amazon Gift Card - Diwali Bonus</v>
       </c>
     </row>
     <row r="283">
@@ -4901,7 +4901,7 @@
         <v>2020-12-19</v>
       </c>
       <c r="B327" t="str">
-        <v>Entertainment</v>
+        <v>Subscriptions</v>
       </c>
       <c r="C327">
         <v>999</v>
@@ -10535,7 +10535,7 @@
         <v>2100</v>
       </c>
       <c r="D732" t="str">
-        <v>Diwali Bonus</v>
+        <v>Amazon Gift Card - Diwali Bonus</v>
       </c>
     </row>
     <row r="733">
@@ -11030,7 +11030,7 @@
         <v>2021-12-12</v>
       </c>
       <c r="B768" t="str">
-        <v>Entertainment</v>
+        <v>Subscriptions</v>
       </c>
       <c r="C768">
         <v>999</v>
@@ -12648,7 +12648,7 @@
     </row>
     <row r="884">
       <c r="A884" t="str">
-        <v>2022-03-22</v>
+        <v>2022-04-11</v>
       </c>
       <c r="B884" t="str">
         <v>Cashback</v>
@@ -14984,9 +14984,3873 @@
         <v>Spotify</v>
       </c>
     </row>
+    <row r="1051">
+      <c r="A1051" t="str">
+        <v>2022-07-30</v>
+      </c>
+      <c r="B1051" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1051">
+        <v>191</v>
+      </c>
+      <c r="D1051" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="str">
+        <v>2022-08-01</v>
+      </c>
+      <c r="B1052" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1052">
+        <v>1081</v>
+      </c>
+      <c r="D1052" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="str">
+        <v>2022-08-01</v>
+      </c>
+      <c r="B1053" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1053">
+        <v>720</v>
+      </c>
+      <c r="D1053" t="str">
+        <v>Bigbasket</v>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="str">
+        <v>2022-08-01</v>
+      </c>
+      <c r="B1054" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1054">
+        <v>70</v>
+      </c>
+      <c r="D1054" t="str">
+        <v>Tender coconut</v>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="str">
+        <v>2022-08-01</v>
+      </c>
+      <c r="B1055" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1055">
+        <v>129</v>
+      </c>
+      <c r="D1055" t="str">
+        <v>Youtube</v>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="str">
+        <v>2022-08-02</v>
+      </c>
+      <c r="B1056" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1056">
+        <v>164</v>
+      </c>
+      <c r="D1056" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="str">
+        <v>2022-08-02</v>
+      </c>
+      <c r="B1057" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1057">
+        <v>90</v>
+      </c>
+      <c r="D1057" t="str">
+        <v>NACH: HCL</v>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="str">
+        <v>2022-08-03</v>
+      </c>
+      <c r="B1058" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1058">
+        <v>596</v>
+      </c>
+      <c r="D1058" t="str">
+        <v>Amazon</v>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="str">
+        <v>2022-08-03</v>
+      </c>
+      <c r="B1059" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1059">
+        <v>208</v>
+      </c>
+      <c r="D1059" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="str">
+        <v>2022-08-03</v>
+      </c>
+      <c r="B1060" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1060">
+        <v>96</v>
+      </c>
+      <c r="D1060" t="str">
+        <v>NACH: TCS</v>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="str">
+        <v>2022-08-02</v>
+      </c>
+      <c r="B1061" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1061">
+        <v>90</v>
+      </c>
+      <c r="D1061" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="str">
+        <v>2022-08-04</v>
+      </c>
+      <c r="B1062" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1062">
+        <v>117</v>
+      </c>
+      <c r="D1062" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="str">
+        <v>2022-08-05</v>
+      </c>
+      <c r="B1063" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1063">
+        <v>144</v>
+      </c>
+      <c r="D1063" t="str">
+        <v xml:space="preserve">Swiggy </v>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="str">
+        <v>2022-08-06</v>
+      </c>
+      <c r="B1064" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C1064">
+        <v>86470</v>
+      </c>
+      <c r="D1064" t="str">
+        <v>Salary for the month of July</v>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="str">
+        <v>2022-08-07</v>
+      </c>
+      <c r="B1065" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1065">
+        <v>140</v>
+      </c>
+      <c r="D1065" t="str">
+        <v>Water and Dairy</v>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="str">
+        <v>2022-08-08</v>
+      </c>
+      <c r="B1066" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1066">
+        <v>604</v>
+      </c>
+      <c r="D1066" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="str">
+        <v>2022-08-08</v>
+      </c>
+      <c r="B1067" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1067">
+        <v>77</v>
+      </c>
+      <c r="D1067" t="str">
+        <v>NACH: Deepak Nitrite</v>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="str">
+        <v>2022-08-08</v>
+      </c>
+      <c r="B1068" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1068">
+        <v>129</v>
+      </c>
+      <c r="D1068" t="str">
+        <v>Amazon</v>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="str">
+        <v>2022-08-08</v>
+      </c>
+      <c r="B1069" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1069">
+        <v>19</v>
+      </c>
+      <c r="D1069" t="str">
+        <v>NACH: Vedanta</v>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="str">
+        <v>2022-08-08</v>
+      </c>
+      <c r="B1070" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1070">
+        <v>420</v>
+      </c>
+      <c r="D1070" t="str">
+        <v>NACH: Tech Mahindra</v>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="str">
+        <v>2022-08-09</v>
+      </c>
+      <c r="B1071" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1071">
+        <v>200</v>
+      </c>
+      <c r="D1071" t="str">
+        <v xml:space="preserve">DDA maintenance </v>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="str">
+        <v>2022-08-12</v>
+      </c>
+      <c r="B1072" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1072">
+        <v>623</v>
+      </c>
+      <c r="D1072" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="str">
+        <v>2022-08-13</v>
+      </c>
+      <c r="B1073" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1073">
+        <v>705</v>
+      </c>
+      <c r="D1073" t="str">
+        <v>Bigbasket</v>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="str">
+        <v>2022-08-13</v>
+      </c>
+      <c r="B1074" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1074">
+        <v>510</v>
+      </c>
+      <c r="D1074" t="str">
+        <v>Petrol</v>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="str">
+        <v>2022-08-14</v>
+      </c>
+      <c r="B1075" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C1075">
+        <v>32</v>
+      </c>
+      <c r="D1075" t="str">
+        <v>Abineesha’s Recharge (50 NPR)</v>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="str">
+        <v>2022-08-16</v>
+      </c>
+      <c r="B1076" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1076">
+        <v>90</v>
+      </c>
+      <c r="D1076" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="str">
+        <v>2022-08-17</v>
+      </c>
+      <c r="B1077" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1077">
+        <v>9000</v>
+      </c>
+      <c r="D1077" t="str">
+        <v>Rent</v>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="str">
+        <v>2022-08-18</v>
+      </c>
+      <c r="B1078" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1078">
+        <v>846</v>
+      </c>
+      <c r="D1078" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="str">
+        <v>2022-08-19</v>
+      </c>
+      <c r="B1079" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1079">
+        <v>90</v>
+      </c>
+      <c r="D1079" t="str">
+        <v>Bike battery charge and wash</v>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="str">
+        <v>2022-08-20</v>
+      </c>
+      <c r="B1080" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1080">
+        <v>240</v>
+      </c>
+      <c r="D1080" t="str">
+        <v>Garbage (May-Aug)</v>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="str">
+        <v>2022-08-21</v>
+      </c>
+      <c r="B1081" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1081">
+        <v>60</v>
+      </c>
+      <c r="D1081" t="str">
+        <v>Coconut Water</v>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="str">
+        <v>2022-08-23</v>
+      </c>
+      <c r="B1082" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1082">
+        <v>90</v>
+      </c>
+      <c r="D1082" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="str">
+        <v>2022-08-24</v>
+      </c>
+      <c r="B1083" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1083">
+        <v>985</v>
+      </c>
+      <c r="D1083" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="str">
+        <v>2022-08-24</v>
+      </c>
+      <c r="B1084" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1084">
+        <v>66</v>
+      </c>
+      <c r="D1084" t="str">
+        <v>NACH: Dr Lal Path Labs</v>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="str">
+        <v>2022-08-25</v>
+      </c>
+      <c r="B1085" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1085">
+        <v>139</v>
+      </c>
+      <c r="D1085" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="str">
+        <v>2022-08-26</v>
+      </c>
+      <c r="B1086" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1086">
+        <v>757</v>
+      </c>
+      <c r="D1086" t="str">
+        <v xml:space="preserve">Bigbasket </v>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="str">
+        <v>2022-08-28</v>
+      </c>
+      <c r="B1087" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1087">
+        <v>142</v>
+      </c>
+      <c r="D1087" t="str">
+        <v>Water and dairy</v>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="str">
+        <v>2022-08-29</v>
+      </c>
+      <c r="B1088" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1088">
+        <v>4076</v>
+      </c>
+      <c r="D1088" t="str">
+        <v>Amazon (Philips trimmer)</v>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="str">
+        <v>2022-08-29</v>
+      </c>
+      <c r="B1089" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1089">
+        <v>209</v>
+      </c>
+      <c r="D1089" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="str">
+        <v>2022-08-29</v>
+      </c>
+      <c r="B1090" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1090">
+        <v>48</v>
+      </c>
+      <c r="D1090" t="str">
+        <v>NACH: Reliance</v>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="str">
+        <v>2022-08-29</v>
+      </c>
+      <c r="B1091" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1091">
+        <v>33</v>
+      </c>
+      <c r="D1091" t="str">
+        <v>NACH: CAM</v>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="str">
+        <v>2022-09-01</v>
+      </c>
+      <c r="B1092" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1092">
+        <v>405</v>
+      </c>
+      <c r="D1092" t="str">
+        <v xml:space="preserve">Amazon </v>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="str">
+        <v>2022-09-01</v>
+      </c>
+      <c r="B1093" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1093">
+        <v>642</v>
+      </c>
+      <c r="D1093" t="str">
+        <v xml:space="preserve">Bigbasket </v>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="str">
+        <v>2022-09-01</v>
+      </c>
+      <c r="B1094" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1094">
+        <v>694</v>
+      </c>
+      <c r="D1094" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="str">
+        <v>2022-09-01</v>
+      </c>
+      <c r="B1095" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1095">
+        <v>129</v>
+      </c>
+      <c r="D1095" t="str">
+        <v>Youtube</v>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="str">
+        <v>2022-09-01</v>
+      </c>
+      <c r="B1096" t="str">
+        <v>Subscriptions</v>
+      </c>
+      <c r="C1096">
+        <v>169</v>
+      </c>
+      <c r="D1096" t="str">
+        <v>Amazon Prime Reading</v>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="str">
+        <v>2022-09-01</v>
+      </c>
+      <c r="B1097" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1097">
+        <v>219</v>
+      </c>
+      <c r="D1097" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="str">
+        <v>2022-09-02</v>
+      </c>
+      <c r="B1098" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1098">
+        <v>117</v>
+      </c>
+      <c r="D1098" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="str">
+        <v>2022-09-04</v>
+      </c>
+      <c r="B1099" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1099">
+        <v>700</v>
+      </c>
+      <c r="D1099" t="str">
+        <v>Bigbasket</v>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="str">
+        <v>2022-09-04</v>
+      </c>
+      <c r="B1100" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1100">
+        <v>137</v>
+      </c>
+      <c r="D1100" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="str">
+        <v>2022-09-06</v>
+      </c>
+      <c r="B1101" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1101">
+        <v>174</v>
+      </c>
+      <c r="D1101" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="str">
+        <v>2022-09-06</v>
+      </c>
+      <c r="B1102" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1102">
+        <v>181</v>
+      </c>
+      <c r="D1102" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="str">
+        <v>2022-09-07</v>
+      </c>
+      <c r="B1103" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C1103">
+        <v>86470</v>
+      </c>
+      <c r="D1103" t="str">
+        <v>Salary for the month August</v>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="str">
+        <v>2022-09-06</v>
+      </c>
+      <c r="B1104" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1104">
+        <v>86</v>
+      </c>
+      <c r="D1104" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="str">
+        <v>2022-09-07</v>
+      </c>
+      <c r="B1105" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1105">
+        <v>82</v>
+      </c>
+      <c r="D1105" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="str">
+        <v>2022-09-07</v>
+      </c>
+      <c r="B1106" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1106">
+        <v>69</v>
+      </c>
+      <c r="D1106" t="str">
+        <v>NACH: Jubliant Foodworks</v>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="str">
+        <v>2022-09-07</v>
+      </c>
+      <c r="B1107" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1107">
+        <v>175</v>
+      </c>
+      <c r="D1107" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="str">
+        <v>2022-09-08</v>
+      </c>
+      <c r="B1108" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1108">
+        <v>200</v>
+      </c>
+      <c r="D1108" t="str">
+        <v>DDA Maintenance</v>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="str">
+        <v>2022-09-08</v>
+      </c>
+      <c r="B1109" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1109">
+        <v>127</v>
+      </c>
+      <c r="D1109" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="str">
+        <v>2022-09-08</v>
+      </c>
+      <c r="B1110" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1110">
+        <v>1200</v>
+      </c>
+      <c r="D1110" t="str">
+        <v>Irctc to Mainpuri</v>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="str">
+        <v>2022-09-09</v>
+      </c>
+      <c r="B1111" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1111">
+        <v>164</v>
+      </c>
+      <c r="D1111" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="str">
+        <v>2022-09-09</v>
+      </c>
+      <c r="B1112" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1112">
+        <v>900</v>
+      </c>
+      <c r="D1112" t="str">
+        <v xml:space="preserve">Bigbasket </v>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="str">
+        <v>2022-09-11</v>
+      </c>
+      <c r="B1113" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1113">
+        <v>355</v>
+      </c>
+      <c r="D1113" t="str">
+        <v xml:space="preserve">Bigbasket </v>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="str">
+        <v>2022-09-11</v>
+      </c>
+      <c r="B1114" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1114">
+        <v>152</v>
+      </c>
+      <c r="D1114" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="str">
+        <v>2022-09-12</v>
+      </c>
+      <c r="B1115" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1115">
+        <v>450</v>
+      </c>
+      <c r="D1115" t="str">
+        <v>Bigbasket</v>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="str">
+        <v>2022-09-13</v>
+      </c>
+      <c r="B1116" t="str">
+        <v>Fitness</v>
+      </c>
+      <c r="C1116">
+        <v>594</v>
+      </c>
+      <c r="D1116" t="str">
+        <v>Papa's Onetouch strips</v>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="str">
+        <v>2022-09-14</v>
+      </c>
+      <c r="B1117" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1117">
+        <v>120</v>
+      </c>
+      <c r="D1117" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="str">
+        <v>2022-09-15</v>
+      </c>
+      <c r="B1118" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1118">
+        <v>132</v>
+      </c>
+      <c r="D1118" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="str">
+        <v>2022-09-15</v>
+      </c>
+      <c r="B1119" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1119">
+        <v>155</v>
+      </c>
+      <c r="D1119" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="str">
+        <v>2022-09-16</v>
+      </c>
+      <c r="B1120" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1120">
+        <v>138</v>
+      </c>
+      <c r="D1120" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="str">
+        <v>2022-09-16</v>
+      </c>
+      <c r="B1121" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1121">
+        <v>206</v>
+      </c>
+      <c r="D1121" t="str">
+        <v>Swiggy Instamart</v>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="str">
+        <v>2022-09-17</v>
+      </c>
+      <c r="B1122" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1122">
+        <v>14</v>
+      </c>
+      <c r="D1122" t="str">
+        <v>NACH: Astral</v>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="str">
+        <v>2022-09-17</v>
+      </c>
+      <c r="B1123" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1123">
+        <v>9000</v>
+      </c>
+      <c r="D1123" t="str">
+        <v>Rent</v>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="str">
+        <v>2022-09-17</v>
+      </c>
+      <c r="B1124" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1124">
+        <v>125</v>
+      </c>
+      <c r="D1124" t="str">
+        <v>Swiggy Instamart</v>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="str">
+        <v>2022-09-18</v>
+      </c>
+      <c r="B1125" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C1125">
+        <v>3002</v>
+      </c>
+      <c r="D1125" t="str">
+        <v>Airtel Wifi Mainpuri 6 months</v>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="str">
+        <v>2022-09-18</v>
+      </c>
+      <c r="B1126" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1126">
+        <v>60</v>
+      </c>
+      <c r="D1126" t="str">
+        <v>Garbage</v>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="str">
+        <v>2022-09-18</v>
+      </c>
+      <c r="B1127" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1127">
+        <v>60</v>
+      </c>
+      <c r="D1127" t="str">
+        <v>Coconut water</v>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="str">
+        <v>2022-09-18</v>
+      </c>
+      <c r="B1128" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1128">
+        <v>92</v>
+      </c>
+      <c r="D1128" t="str">
+        <v>Water and dairy</v>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="str">
+        <v>2022-09-19</v>
+      </c>
+      <c r="B1129" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1129">
+        <v>72</v>
+      </c>
+      <c r="D1129" t="str">
+        <v>NACH: IRCTC</v>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="str">
+        <v>2022-09-19</v>
+      </c>
+      <c r="B1130" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1130">
+        <v>970</v>
+      </c>
+      <c r="D1130" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="str">
+        <v>2022-09-21</v>
+      </c>
+      <c r="B1131" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1131">
+        <v>239</v>
+      </c>
+      <c r="D1131" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="str">
+        <v>2022-09-23</v>
+      </c>
+      <c r="B1132" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1132">
+        <v>159</v>
+      </c>
+      <c r="D1132" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="str">
+        <v>2022-09-24</v>
+      </c>
+      <c r="B1133" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1133">
+        <v>199</v>
+      </c>
+      <c r="D1133" t="str">
+        <v>Amazon</v>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="str">
+        <v>2022-09-24</v>
+      </c>
+      <c r="B1134" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1134">
+        <v>90</v>
+      </c>
+      <c r="D1134" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="str">
+        <v>2022-09-25</v>
+      </c>
+      <c r="B1135" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1135">
+        <v>656</v>
+      </c>
+      <c r="D1135" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="str">
+        <v>2022-09-26</v>
+      </c>
+      <c r="B1136" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1136">
+        <v>143</v>
+      </c>
+      <c r="D1136" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="str">
+        <v>2022-09-27</v>
+      </c>
+      <c r="B1137" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1137">
+        <v>1000</v>
+      </c>
+      <c r="D1137" t="str">
+        <v>Birthday gift from Neeraj Bhaiya</v>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="str">
+        <v>2022-09-27</v>
+      </c>
+      <c r="B1138" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1138">
+        <v>213</v>
+      </c>
+      <c r="D1138" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="str">
+        <v>2022-09-25</v>
+      </c>
+      <c r="B1139" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1139">
+        <v>101</v>
+      </c>
+      <c r="D1139" t="str">
+        <v xml:space="preserve">SBI Credit Interest </v>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="str">
+        <v>2022-09-29</v>
+      </c>
+      <c r="B1140" t="str">
+        <v/>
+      </c>
+      <c r="C1140">
+        <v>3125</v>
+      </c>
+      <c r="D1140" t="str">
+        <v>To Abineesha</v>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="str">
+        <v>2022-09-29</v>
+      </c>
+      <c r="B1141" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1141">
+        <v>315</v>
+      </c>
+      <c r="D1141" t="str">
+        <v>Amazon Cashback</v>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="str">
+        <v>2022-09-29</v>
+      </c>
+      <c r="B1142" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1142">
+        <v>138</v>
+      </c>
+      <c r="D1142" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="str">
+        <v>2022-09-30</v>
+      </c>
+      <c r="B1143" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1143">
+        <v>152</v>
+      </c>
+      <c r="D1143" t="str">
+        <v>Water and Dairy</v>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="str">
+        <v>2022-09-30</v>
+      </c>
+      <c r="B1144" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1144">
+        <v>143</v>
+      </c>
+      <c r="D1144" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="str">
+        <v>2022-10-01</v>
+      </c>
+      <c r="B1145" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1145">
+        <v>129</v>
+      </c>
+      <c r="D1145" t="str">
+        <v>Youtube</v>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="str">
+        <v>2022-10-02</v>
+      </c>
+      <c r="B1146" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1146">
+        <v>216</v>
+      </c>
+      <c r="D1146" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="str">
+        <v>2022-10-02</v>
+      </c>
+      <c r="B1147" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1147">
+        <v>157</v>
+      </c>
+      <c r="D1147" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="str">
+        <v>2022-10-03</v>
+      </c>
+      <c r="B1148" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1148">
+        <v>490</v>
+      </c>
+      <c r="D1148" t="str">
+        <v>Bigbasket</v>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="str">
+        <v>2022-10-03</v>
+      </c>
+      <c r="B1149" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1149">
+        <v>610</v>
+      </c>
+      <c r="D1149" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="str">
+        <v>2022-10-04</v>
+      </c>
+      <c r="B1150" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1150">
+        <v>3090</v>
+      </c>
+      <c r="D1150" t="str">
+        <v>UBI Credit Interest</v>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="str">
+        <v>2022-10-05</v>
+      </c>
+      <c r="B1151" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1151">
+        <v>86</v>
+      </c>
+      <c r="D1151" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="str">
+        <v>2022-10-06</v>
+      </c>
+      <c r="B1152" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1152">
+        <v>134</v>
+      </c>
+      <c r="D1152" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="str">
+        <v>2022-10-06</v>
+      </c>
+      <c r="B1153" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1153">
+        <v>149</v>
+      </c>
+      <c r="D1153" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="str">
+        <v>2022-10-07</v>
+      </c>
+      <c r="B1154" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C1154">
+        <v>86470</v>
+      </c>
+      <c r="D1154" t="str">
+        <v>Salary for the month of Sept</v>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="str">
+        <v>2022-10-07</v>
+      </c>
+      <c r="B1155" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1155">
+        <v>90</v>
+      </c>
+      <c r="D1155" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="str">
+        <v>2022-10-07</v>
+      </c>
+      <c r="B1156" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1156">
+        <v>119</v>
+      </c>
+      <c r="D1156" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="str">
+        <v>2022-10-07</v>
+      </c>
+      <c r="B1157" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1157">
+        <v>1268</v>
+      </c>
+      <c r="D1157" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="str">
+        <v>2022-10-09</v>
+      </c>
+      <c r="B1158" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1158">
+        <v>86</v>
+      </c>
+      <c r="D1158" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="str">
+        <v>2022-10-10</v>
+      </c>
+      <c r="B1159" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1159">
+        <v>138</v>
+      </c>
+      <c r="D1159" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="str">
+        <v>2022-10-10</v>
+      </c>
+      <c r="B1160" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1160">
+        <v>200</v>
+      </c>
+      <c r="D1160" t="str">
+        <v xml:space="preserve">DDA Maintenance </v>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="str">
+        <v>2022-10-11</v>
+      </c>
+      <c r="B1161" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1161">
+        <v>302</v>
+      </c>
+      <c r="D1161" t="str">
+        <v>Swiggy Instamart</v>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="str">
+        <v>2022-10-11</v>
+      </c>
+      <c r="B1162" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1162">
+        <v>351</v>
+      </c>
+      <c r="D1162" t="str">
+        <v>Swiggy Instamart</v>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="str">
+        <v>2022-05-11</v>
+      </c>
+      <c r="B1163" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1163">
+        <v>433</v>
+      </c>
+      <c r="D1163" t="str">
+        <v>Flipkart Cashback</v>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="str">
+        <v>2022-06-10</v>
+      </c>
+      <c r="B1164" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1164">
+        <v>119</v>
+      </c>
+      <c r="D1164" t="str">
+        <v>Flipkart Cashback</v>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="str">
+        <v>2022-07-11</v>
+      </c>
+      <c r="B1165" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1165">
+        <v>121</v>
+      </c>
+      <c r="D1165" t="str">
+        <v>Flipkart Cashback</v>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="str">
+        <v>2022-08-10</v>
+      </c>
+      <c r="B1166" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1166">
+        <v>171</v>
+      </c>
+      <c r="D1166" t="str">
+        <v>Flipkart Cashback</v>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="str">
+        <v>2022-09-12</v>
+      </c>
+      <c r="B1167" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1167">
+        <v>241</v>
+      </c>
+      <c r="D1167" t="str">
+        <v>Flipkart Cashback</v>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="str">
+        <v>2022-10-11</v>
+      </c>
+      <c r="B1168" t="str">
+        <v>Cashback</v>
+      </c>
+      <c r="C1168">
+        <v>56</v>
+      </c>
+      <c r="D1168" t="str">
+        <v>Flipkart Cashback</v>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="str">
+        <v>2022-10-13</v>
+      </c>
+      <c r="B1169" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1169">
+        <v>138</v>
+      </c>
+      <c r="D1169" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="str">
+        <v>2022-10-13</v>
+      </c>
+      <c r="B1170" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1170">
+        <v>90</v>
+      </c>
+      <c r="D1170" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="str">
+        <v>2022-10-16</v>
+      </c>
+      <c r="B1171" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1171">
+        <v>400</v>
+      </c>
+      <c r="D1171" t="str">
+        <v>Ola Cab and E-rickshaw</v>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="str">
+        <v>2022-10-17</v>
+      </c>
+      <c r="B1172" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1172">
+        <v>9000</v>
+      </c>
+      <c r="D1172" t="str">
+        <v>Rent</v>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="str">
+        <v>2022-10-17</v>
+      </c>
+      <c r="B1173" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1173">
+        <v>295</v>
+      </c>
+      <c r="D1173" t="str">
+        <v xml:space="preserve">Amazon </v>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="str">
+        <v>2022-10-17</v>
+      </c>
+      <c r="B1174" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1174">
+        <v>349</v>
+      </c>
+      <c r="D1174" t="str">
+        <v>Amazon, earphones for papa</v>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="str">
+        <v>2022-10-17</v>
+      </c>
+      <c r="B1175" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1175">
+        <v>349</v>
+      </c>
+      <c r="D1175" t="str">
+        <v>Amazon rangoli colors</v>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="str">
+        <v>2022-10-18</v>
+      </c>
+      <c r="B1176" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1176">
+        <v>149</v>
+      </c>
+      <c r="D1176" t="str">
+        <v>Amazon screen guard for poco c3</v>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="str">
+        <v>2022-10-20</v>
+      </c>
+      <c r="B1177" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C1177">
+        <v>150</v>
+      </c>
+      <c r="D1177" t="str">
+        <v>Apple iCloud subscription</v>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="str">
+        <v>2022-10-20</v>
+      </c>
+      <c r="B1178" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1178">
+        <v>2100</v>
+      </c>
+      <c r="D1178" t="str">
+        <v>Amazon Gift Card - Diwali Bonus</v>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="str">
+        <v>2022-10-20</v>
+      </c>
+      <c r="B1179" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1179">
+        <v>2950</v>
+      </c>
+      <c r="D1179" t="str">
+        <v>Amazon: Biometric fingerprint sensor for papa</v>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="str">
+        <v>2022-10-23</v>
+      </c>
+      <c r="B1180" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1180">
+        <v>149</v>
+      </c>
+      <c r="D1180" t="str">
+        <v>Samsung M21 screen guard</v>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="str">
+        <v>2022-10-27</v>
+      </c>
+      <c r="B1181" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1181">
+        <v>10000</v>
+      </c>
+      <c r="D1181" t="str">
+        <v>Diwali shopping (clothes for everyone)</v>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="str">
+        <v>2022-10-28</v>
+      </c>
+      <c r="B1182" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1182">
+        <v>119</v>
+      </c>
+      <c r="D1182" t="str">
+        <v>Spotify</v>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="str">
+        <v>2022-10-30</v>
+      </c>
+      <c r="B1183" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C1183">
+        <v>100</v>
+      </c>
+      <c r="D1183" t="str">
+        <v>Nepal Telecom Recharge</v>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="str">
+        <v>2022-10-30</v>
+      </c>
+      <c r="B1184" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1184">
+        <v>332</v>
+      </c>
+      <c r="D1184" t="str">
+        <v>Amazon water overflow alarm</v>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="str">
+        <v>2022-11-01</v>
+      </c>
+      <c r="B1185" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1185">
+        <v>13456</v>
+      </c>
+      <c r="D1185" t="str">
+        <v>Trip to Ktm and return flight</v>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="str">
+        <v>2022-10-31</v>
+      </c>
+      <c r="B1186" t="str">
+        <v>Cashback</v>
+      </c>
+      <c r="C1186">
+        <v>229</v>
+      </c>
+      <c r="D1186" t="str">
+        <v>Amazon cashback</v>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="str">
+        <v>2022-11-01</v>
+      </c>
+      <c r="B1187" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1187">
+        <v>129</v>
+      </c>
+      <c r="D1187" t="str">
+        <v xml:space="preserve">YouTube </v>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="str">
+        <v>2022-11-02</v>
+      </c>
+      <c r="B1188" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1188">
+        <v>90</v>
+      </c>
+      <c r="D1188" t="str">
+        <v>NACH: HCL</v>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="str">
+        <v>2022-11-06</v>
+      </c>
+      <c r="B1189" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C1189">
+        <v>86470</v>
+      </c>
+      <c r="D1189" t="str">
+        <v>Salary for the month October</v>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="str">
+        <v>2022-11-06</v>
+      </c>
+      <c r="B1190" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1190">
+        <v>1199</v>
+      </c>
+      <c r="D1190" t="str">
+        <v>Irctc to Delhi</v>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="str">
+        <v>2022-11-07</v>
+      </c>
+      <c r="B1191" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1191">
+        <v>104</v>
+      </c>
+      <c r="D1191" t="str">
+        <v>NACH: TCS</v>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="str">
+        <v>2022-11-10</v>
+      </c>
+      <c r="B1192" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1192">
+        <v>495</v>
+      </c>
+      <c r="D1192" t="str">
+        <v>NACH: Infosys</v>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="str">
+        <v>2022-11-10</v>
+      </c>
+      <c r="B1193" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1193">
+        <v>88</v>
+      </c>
+      <c r="D1193" t="str">
+        <v>NACH: Asian Paints</v>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="str">
+        <v>2022-11-11</v>
+      </c>
+      <c r="B1194" t="str">
+        <v>Cashback</v>
+      </c>
+      <c r="C1194">
+        <v>113</v>
+      </c>
+      <c r="D1194" t="str">
+        <v>Flipkart Cashback</v>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="str">
+        <v>2022-11-13</v>
+      </c>
+      <c r="B1195" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1195">
+        <v>50</v>
+      </c>
+      <c r="D1195" t="str">
+        <v>E-rickshaw</v>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="str">
+        <v>2022-11-13</v>
+      </c>
+      <c r="B1196" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1196">
+        <v>164</v>
+      </c>
+      <c r="D1196" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="str">
+        <v>2022-11-13</v>
+      </c>
+      <c r="B1197" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1197">
+        <v>297</v>
+      </c>
+      <c r="D1197" t="str">
+        <v>Swiggy Instamart</v>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="str">
+        <v>2022-11-14</v>
+      </c>
+      <c r="B1198" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1198">
+        <v>138</v>
+      </c>
+      <c r="D1198" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="str">
+        <v>2022-11-16</v>
+      </c>
+      <c r="B1199" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1199">
+        <v>82</v>
+      </c>
+      <c r="D1199" t="str">
+        <v xml:space="preserve">Swiggy </v>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="str">
+        <v>2022-11-16</v>
+      </c>
+      <c r="B1200" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1200">
+        <v>90</v>
+      </c>
+      <c r="D1200" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="str">
+        <v>2022-11-16</v>
+      </c>
+      <c r="B1201" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1201">
+        <v>1446</v>
+      </c>
+      <c r="D1201" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="str">
+        <v>2022-11-17</v>
+      </c>
+      <c r="B1202" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1202">
+        <v>170</v>
+      </c>
+      <c r="D1202" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="str">
+        <v>2022-11-17</v>
+      </c>
+      <c r="B1203" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1203">
+        <v>9000</v>
+      </c>
+      <c r="D1203" t="str">
+        <v>Rent</v>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="str">
+        <v>2022-11-18</v>
+      </c>
+      <c r="B1204" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1204">
+        <v>120</v>
+      </c>
+      <c r="D1204" t="str">
+        <v>Garbage</v>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="str">
+        <v>2022-11-19</v>
+      </c>
+      <c r="B1205" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1205">
+        <v>2947</v>
+      </c>
+      <c r="D1205" t="str">
+        <v>Delhi to Kathmandu Flight Reschedule</v>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="str">
+        <v>2022-11-19</v>
+      </c>
+      <c r="B1206" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1206">
+        <v>150</v>
+      </c>
+      <c r="D1206" t="str">
+        <v>Flight Seat selection</v>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="str">
+        <v>2022-11-19</v>
+      </c>
+      <c r="B1207" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1207">
+        <v>320</v>
+      </c>
+      <c r="D1207" t="str">
+        <v>Uber</v>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="str">
+        <v>2022-11-20</v>
+      </c>
+      <c r="B1208" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1208">
+        <v>153</v>
+      </c>
+      <c r="D1208" t="str">
+        <v xml:space="preserve">Swiggy </v>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="str">
+        <v>2022-11-20</v>
+      </c>
+      <c r="B1209" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1209">
+        <v>100</v>
+      </c>
+      <c r="D1209" t="str">
+        <v xml:space="preserve">Metro Card Recharge </v>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="str">
+        <v>2022-11-20</v>
+      </c>
+      <c r="B1210" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1210">
+        <v>1999</v>
+      </c>
+      <c r="D1210" t="str">
+        <v>Oneplus Wireless Z Earphones</v>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="str">
+        <v>2022-11-21</v>
+      </c>
+      <c r="B1211" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1211">
+        <v>132</v>
+      </c>
+      <c r="D1211" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="str">
+        <v>2022-11-22</v>
+      </c>
+      <c r="B1212" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1212">
+        <v>94</v>
+      </c>
+      <c r="D1212" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="str">
+        <v>2022-11-22</v>
+      </c>
+      <c r="B1213" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1213">
+        <v>249</v>
+      </c>
+      <c r="D1213" t="str">
+        <v>Amazon Shopping Mouse</v>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="str">
+        <v>2022-11-22</v>
+      </c>
+      <c r="B1214" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1214">
+        <v>131</v>
+      </c>
+      <c r="D1214" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="str">
+        <v>2022-11-23</v>
+      </c>
+      <c r="B1215" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1215">
+        <v>132</v>
+      </c>
+      <c r="D1215" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="str">
+        <v>2022-11-23</v>
+      </c>
+      <c r="B1216" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1216">
+        <v>130</v>
+      </c>
+      <c r="D1216" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="str">
+        <v>2022-11-24</v>
+      </c>
+      <c r="B1217" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1217">
+        <v>72</v>
+      </c>
+      <c r="D1217" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="str">
+        <v>2022-11-24</v>
+      </c>
+      <c r="B1218" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1218">
+        <v>252</v>
+      </c>
+      <c r="D1218" t="str">
+        <v>NACH: Tech Mahindra</v>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="str">
+        <v>2022-11-25</v>
+      </c>
+      <c r="B1219" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1219">
+        <v>216</v>
+      </c>
+      <c r="D1219" t="str">
+        <v xml:space="preserve">Swiggy </v>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="str">
+        <v>2022-11-27</v>
+      </c>
+      <c r="B1220" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1220">
+        <v>960</v>
+      </c>
+      <c r="D1220" t="str">
+        <v>Bike's new battery (Amron) and wash</v>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="str">
+        <v>2022-11-27</v>
+      </c>
+      <c r="B1221" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1221">
+        <v>90</v>
+      </c>
+      <c r="D1221" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="str">
+        <v>2022-11-28</v>
+      </c>
+      <c r="B1222" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1222">
+        <v>132</v>
+      </c>
+      <c r="D1222" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="str">
+        <v>2022-11-28</v>
+      </c>
+      <c r="B1223" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1223">
+        <v>42</v>
+      </c>
+      <c r="D1223" t="str">
+        <v>NACH: CAM</v>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="str">
+        <v>2022-11-28</v>
+      </c>
+      <c r="B1224" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1224">
+        <v>374</v>
+      </c>
+      <c r="D1224" t="str">
+        <v xml:space="preserve">Swiggy Instamart </v>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="str">
+        <v>2022-11-28</v>
+      </c>
+      <c r="B1225" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1225">
+        <v>119</v>
+      </c>
+      <c r="D1225" t="str">
+        <v>Spotify</v>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="str">
+        <v>2022-09-28</v>
+      </c>
+      <c r="B1226" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1226">
+        <v>119</v>
+      </c>
+      <c r="D1226" t="str">
+        <v>Spotify</v>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="str">
+        <v>2022-08-28</v>
+      </c>
+      <c r="B1227" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1227">
+        <v>119</v>
+      </c>
+      <c r="D1227" t="str">
+        <v>Spotify</v>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="str">
+        <v>2022-11-29</v>
+      </c>
+      <c r="B1228" t="str">
+        <v>Cashback</v>
+      </c>
+      <c r="C1228">
+        <v>159</v>
+      </c>
+      <c r="D1228" t="str">
+        <v>Amazon Pay Cashback</v>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="str">
+        <v>2022-11-29</v>
+      </c>
+      <c r="B1229" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1229">
+        <v>155</v>
+      </c>
+      <c r="D1229" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="str">
+        <v>2022-11-30</v>
+      </c>
+      <c r="B1230" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1230">
+        <v>157</v>
+      </c>
+      <c r="D1230" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="str">
+        <v>2022-12-01</v>
+      </c>
+      <c r="B1231" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1231">
+        <v>97</v>
+      </c>
+      <c r="D1231" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="str">
+        <v>2022-12-01</v>
+      </c>
+      <c r="B1232" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1232">
+        <v>129</v>
+      </c>
+      <c r="D1232" t="str">
+        <v xml:space="preserve">YouTube Subscription </v>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="str">
+        <v>2022-12-03</v>
+      </c>
+      <c r="B1233" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1233">
+        <v>132</v>
+      </c>
+      <c r="D1233" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="str">
+        <v>2022-12-03</v>
+      </c>
+      <c r="B1234" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1234">
+        <v>90</v>
+      </c>
+      <c r="D1234" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="str">
+        <v>2022-12-03</v>
+      </c>
+      <c r="B1235" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1235">
+        <v>319</v>
+      </c>
+      <c r="D1235" t="str">
+        <v>Swiggy Instamart</v>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="str">
+        <v>2022-12-04</v>
+      </c>
+      <c r="B1236" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1236">
+        <v>98</v>
+      </c>
+      <c r="D1236" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="str">
+        <v>2022-12-04</v>
+      </c>
+      <c r="B1237" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1237">
+        <v>500</v>
+      </c>
+      <c r="D1237" t="str">
+        <v>Bigbasket BB Daily</v>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="str">
+        <v>2022-12-05</v>
+      </c>
+      <c r="B1238" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1238">
+        <v>375</v>
+      </c>
+      <c r="D1238" t="str">
+        <v>Flipkart shopping slippers</v>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="str">
+        <v>2022-12-06</v>
+      </c>
+      <c r="B1239" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1239">
+        <v>132</v>
+      </c>
+      <c r="D1239" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="str">
+        <v>2022-12-07</v>
+      </c>
+      <c r="B1240" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C1240">
+        <v>86470</v>
+      </c>
+      <c r="D1240" t="str">
+        <v xml:space="preserve">Salary for the month of November </v>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="str">
+        <v>2022-12-06</v>
+      </c>
+      <c r="B1241" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1241">
+        <v>156</v>
+      </c>
+      <c r="D1241" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="str">
+        <v>2022-12-07</v>
+      </c>
+      <c r="B1242" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1242">
+        <v>147</v>
+      </c>
+      <c r="D1242" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="str">
+        <v>2022-12-07</v>
+      </c>
+      <c r="B1243" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1243">
+        <v>182</v>
+      </c>
+      <c r="D1243" t="str">
+        <v>Bigbasket</v>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="str">
+        <v>2022-12-09</v>
+      </c>
+      <c r="B1244" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1244">
+        <v>159</v>
+      </c>
+      <c r="D1244" t="str">
+        <v xml:space="preserve">Swiggy </v>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="str">
+        <v>2022-12-09</v>
+      </c>
+      <c r="B1245" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1245">
+        <v>156</v>
+      </c>
+      <c r="D1245" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="str">
+        <v>2022-12-10</v>
+      </c>
+      <c r="B1246" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1246">
+        <v>90</v>
+      </c>
+      <c r="D1246" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="str">
+        <v>2022-12-10</v>
+      </c>
+      <c r="B1247" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1247">
+        <v>1000</v>
+      </c>
+      <c r="D1247" t="str">
+        <v>Bigbasket BB Daily</v>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="str">
+        <v>2022-12-11</v>
+      </c>
+      <c r="B1248" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1248">
+        <v>86</v>
+      </c>
+      <c r="D1248" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="str">
+        <v>2022-12-11</v>
+      </c>
+      <c r="B1249" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1249">
+        <v>165</v>
+      </c>
+      <c r="D1249" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="str">
+        <v>2022-12-12</v>
+      </c>
+      <c r="B1250" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1250">
+        <v>400</v>
+      </c>
+      <c r="D1250" t="str">
+        <v xml:space="preserve">DDA Maintenance </v>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="str">
+        <v>2022-12-12</v>
+      </c>
+      <c r="B1251" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1251">
+        <v>93</v>
+      </c>
+      <c r="D1251" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="str">
+        <v>2022-12-12</v>
+      </c>
+      <c r="B1252" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1252">
+        <v>138</v>
+      </c>
+      <c r="D1252" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="str">
+        <v>2022-12-13</v>
+      </c>
+      <c r="B1253" t="str">
+        <v>Subscriptions</v>
+      </c>
+      <c r="C1253">
+        <v>1499</v>
+      </c>
+      <c r="D1253" t="str">
+        <v>Amazon Prime</v>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="str">
+        <v>2022-12-13</v>
+      </c>
+      <c r="B1254" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1254">
+        <v>777</v>
+      </c>
+      <c r="D1254" t="str">
+        <v>Amazon (shopping bag, redmi note 7 pro back cover and screen guard, bath towel)</v>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="str">
+        <v>2022-12-13</v>
+      </c>
+      <c r="B1255" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1255">
+        <v>136</v>
+      </c>
+      <c r="D1255" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="str">
+        <v>2022-12-13</v>
+      </c>
+      <c r="B1256" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1256">
+        <v>138</v>
+      </c>
+      <c r="D1256" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="str">
+        <v>2022-12-13</v>
+      </c>
+      <c r="B1257" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1257">
+        <v>52</v>
+      </c>
+      <c r="D1257" t="str">
+        <v>NACH: Vedanta</v>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="str">
+        <v>2022-12-14</v>
+      </c>
+      <c r="B1258" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1258">
+        <v>143</v>
+      </c>
+      <c r="D1258" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="str">
+        <v>2022-12-15</v>
+      </c>
+      <c r="B1259" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1259">
+        <v>392</v>
+      </c>
+      <c r="D1259" t="str">
+        <v>Bigbasket</v>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="str">
+        <v>2022-12-16</v>
+      </c>
+      <c r="B1260" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1260">
+        <v>90</v>
+      </c>
+      <c r="D1260" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="str">
+        <v>2022-12-17</v>
+      </c>
+      <c r="B1261" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1261">
+        <v>9000</v>
+      </c>
+      <c r="D1261" t="str">
+        <v>Rent</v>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="str">
+        <v>2022-12-18</v>
+      </c>
+      <c r="B1262" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1262">
+        <v>439</v>
+      </c>
+      <c r="D1262" t="str">
+        <v>Swiggy Instamart</v>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="str">
+        <v>2022-12-19</v>
+      </c>
+      <c r="B1263" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1263">
+        <v>149</v>
+      </c>
+      <c r="D1263" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="str">
+        <v>2022-12-19</v>
+      </c>
+      <c r="B1264" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1264">
+        <v>102</v>
+      </c>
+      <c r="D1264" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="str">
+        <v>2022-12-19</v>
+      </c>
+      <c r="B1265" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1265">
+        <v>109</v>
+      </c>
+      <c r="D1265" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="str">
+        <v>2022-12-19</v>
+      </c>
+      <c r="B1266" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1266">
+        <v>60</v>
+      </c>
+      <c r="D1266" t="str">
+        <v>Garbage</v>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="str">
+        <v>2022-12-19</v>
+      </c>
+      <c r="B1267" t="str">
+        <v>Vacation</v>
+      </c>
+      <c r="C1267">
+        <v>12197</v>
+      </c>
+      <c r="D1267" t="str">
+        <v>Flight to Kathmandu and return (31st dec - 4th jan)</v>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="str">
+        <v>2022-12-19</v>
+      </c>
+      <c r="B1268" t="str">
+        <v>Vacation</v>
+      </c>
+      <c r="C1268">
+        <v>7195</v>
+      </c>
+      <c r="D1268" t="str">
+        <v>Homestay Airbnb</v>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="str">
+        <v>2022-12-20</v>
+      </c>
+      <c r="B1269" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1269">
+        <v>138</v>
+      </c>
+      <c r="D1269" t="str">
+        <v xml:space="preserve">Swiggy </v>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="str">
+        <v>2022-12-21</v>
+      </c>
+      <c r="B1270" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1270">
+        <v>86</v>
+      </c>
+      <c r="D1270" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="str">
+        <v>2022-12-21</v>
+      </c>
+      <c r="B1271" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1271">
+        <v>3492</v>
+      </c>
+      <c r="D1271" t="str">
+        <v>Myntra</v>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="str">
+        <v>2022-12-21</v>
+      </c>
+      <c r="B1272" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1272">
+        <v>137</v>
+      </c>
+      <c r="D1272" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="str">
+        <v>2022-12-21</v>
+      </c>
+      <c r="B1273" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1273">
+        <v>126</v>
+      </c>
+      <c r="D1273" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="str">
+        <v>2022-12-22</v>
+      </c>
+      <c r="B1274" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1274">
+        <v>86</v>
+      </c>
+      <c r="D1274" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="str">
+        <v>2022-12-22</v>
+      </c>
+      <c r="B1275" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1275">
+        <v>86</v>
+      </c>
+      <c r="D1275" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="str">
+        <v>2022-12-22</v>
+      </c>
+      <c r="B1276" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1276">
+        <v>168</v>
+      </c>
+      <c r="D1276" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="str">
+        <v>2022-12-23</v>
+      </c>
+      <c r="B1277" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1277">
+        <v>86990</v>
+      </c>
+      <c r="D1277" t="str">
+        <v>Apple Macbook Air M1</v>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="str">
+        <v>2022-12-23</v>
+      </c>
+      <c r="B1278" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1278">
+        <v>1199</v>
+      </c>
+      <c r="D1278" t="str">
+        <v>Macbook hub adapter</v>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="str">
+        <v>2022-12-23</v>
+      </c>
+      <c r="B1279" t="str">
+        <v>Investment</v>
+      </c>
+      <c r="C1279">
+        <v>200</v>
+      </c>
+      <c r="D1279" t="str">
+        <v>Zerodha account opening fee</v>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="str">
+        <v>2022-12-23</v>
+      </c>
+      <c r="B1280" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1280">
+        <v>130</v>
+      </c>
+      <c r="D1280" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="str">
+        <v>2022-12-23</v>
+      </c>
+      <c r="B1281" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1281">
+        <v>158</v>
+      </c>
+      <c r="D1281" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="str">
+        <v>2022-12-24</v>
+      </c>
+      <c r="B1282" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1282">
+        <v>649</v>
+      </c>
+      <c r="D1282" t="str">
+        <v>Netflix</v>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="str">
+        <v>2022-12-24</v>
+      </c>
+      <c r="B1283" t="str">
+        <v>HealthCare</v>
+      </c>
+      <c r="C1283">
+        <v>1098</v>
+      </c>
+      <c r="D1283" t="str">
+        <v>Apollo Papa's test</v>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="str">
+        <v>2022-12-24</v>
+      </c>
+      <c r="B1284" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1284">
+        <v>301</v>
+      </c>
+      <c r="D1284" t="str">
+        <v>Swiggy Instamart</v>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="str">
+        <v>2022-12-24</v>
+      </c>
+      <c r="B1285" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1285">
+        <v>812</v>
+      </c>
+      <c r="D1285" t="str">
+        <v>Flipkart Abineesha's clothes</v>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="str">
+        <v>2022-12-24</v>
+      </c>
+      <c r="B1286" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1286">
+        <v>86</v>
+      </c>
+      <c r="D1286" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="str">
+        <v>2022-12-26</v>
+      </c>
+      <c r="B1287" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1287">
+        <v>3301</v>
+      </c>
+      <c r="D1287" t="str">
+        <v>Myntra</v>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="str">
+        <v>2022-12-26</v>
+      </c>
+      <c r="B1288" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C1288">
+        <v>455</v>
+      </c>
+      <c r="D1288" t="str">
+        <v>Airtel Bill 3 months plan</v>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="str">
+        <v>2022-12-26</v>
+      </c>
+      <c r="B1289" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1289">
+        <v>180</v>
+      </c>
+      <c r="D1289" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="str">
+        <v>2022-12-26</v>
+      </c>
+      <c r="B1290" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1290">
+        <v>200</v>
+      </c>
+      <c r="D1290" t="str">
+        <v xml:space="preserve">Swiggy Instamart </v>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="str">
+        <v>2022-12-27</v>
+      </c>
+      <c r="B1291" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1291">
+        <v>1099</v>
+      </c>
+      <c r="D1291" t="str">
+        <v>Offbeat dash wireless bluetooth mouse</v>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="str">
+        <v>2022-12-28</v>
+      </c>
+      <c r="B1292" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1292">
+        <v>312</v>
+      </c>
+      <c r="D1292" t="str">
+        <v>Irctc to Etawah (mom dad)</v>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="str">
+        <v>2022-12-28</v>
+      </c>
+      <c r="B1293" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1293">
+        <v>119</v>
+      </c>
+      <c r="D1293" t="str">
+        <v>Spotify</v>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="str">
+        <v>2022-12-28</v>
+      </c>
+      <c r="B1294" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1294">
+        <v>434</v>
+      </c>
+      <c r="D1294" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="str">
+        <v>2022-12-30</v>
+      </c>
+      <c r="B1295" t="str">
+        <v>Cashback</v>
+      </c>
+      <c r="C1295">
+        <v>4712</v>
+      </c>
+      <c r="D1295" t="str">
+        <v>Amazon Cashback</v>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="B1296" t="str">
+        <v>Entertainment</v>
+      </c>
+      <c r="C1296">
+        <v>129</v>
+      </c>
+      <c r="D1296" t="str">
+        <v>Youtube Subscription</v>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="str">
+        <v>2023-01-01</v>
+      </c>
+      <c r="B1297" t="str">
+        <v>Transportation</v>
+      </c>
+      <c r="C1297">
+        <v>290</v>
+      </c>
+      <c r="D1297" t="str">
+        <v>Uber</v>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="str">
+        <v>2022-12-27</v>
+      </c>
+      <c r="B1298" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1298">
+        <v>349</v>
+      </c>
+      <c r="D1298" t="str">
+        <v>Flipkart</v>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="str">
+        <v>2023-01-04</v>
+      </c>
+      <c r="B1299" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1299">
+        <v>132</v>
+      </c>
+      <c r="D1299" t="str">
+        <v xml:space="preserve">Swiggy </v>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="str">
+        <v>2023-01-05</v>
+      </c>
+      <c r="B1300" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1300">
+        <v>576</v>
+      </c>
+      <c r="D1300" t="str">
+        <v>Swiggy Instamart</v>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="str">
+        <v>2023-01-05</v>
+      </c>
+      <c r="B1301" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1301">
+        <v>4289</v>
+      </c>
+      <c r="D1301" t="str">
+        <v>UBI Credit Interest</v>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="str">
+        <v>2023-01-05</v>
+      </c>
+      <c r="B1302" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1302">
+        <v>86</v>
+      </c>
+      <c r="D1302" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="str">
+        <v>2023-01-07</v>
+      </c>
+      <c r="B1303" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C1303">
+        <v>86470</v>
+      </c>
+      <c r="D1303" t="str">
+        <v>Salary for the month December</v>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="str">
+        <v>2023-01-07</v>
+      </c>
+      <c r="B1304" t="str">
+        <v>Other Income</v>
+      </c>
+      <c r="C1304">
+        <v>2638</v>
+      </c>
+      <c r="D1304" t="str">
+        <v>NACH: LTIMindtree</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="str">
+        <v>2023-01-07</v>
+      </c>
+      <c r="B1305" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1305">
+        <v>200</v>
+      </c>
+      <c r="D1305" t="str">
+        <v>DDA Maintenance</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="str">
+        <v>2023-01-07</v>
+      </c>
+      <c r="B1306" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1306">
+        <v>90</v>
+      </c>
+      <c r="D1306" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="str">
+        <v>2023-01-08</v>
+      </c>
+      <c r="B1307" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1307">
+        <v>161</v>
+      </c>
+      <c r="D1307" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="str">
+        <v>2023-01-09</v>
+      </c>
+      <c r="B1308" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1308">
+        <v>132</v>
+      </c>
+      <c r="D1308" t="str">
+        <v xml:space="preserve">Swiggy </v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="str">
+        <v>2023-01-09</v>
+      </c>
+      <c r="B1309" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C1309">
+        <v>1053</v>
+      </c>
+      <c r="D1309" t="str">
+        <v>LPG Cylinder</v>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="str">
+        <v>2023-01-09</v>
+      </c>
+      <c r="B1310" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1310">
+        <v>147</v>
+      </c>
+      <c r="D1310" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="str">
+        <v>2023-01-10</v>
+      </c>
+      <c r="B1311" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1311">
+        <v>318</v>
+      </c>
+      <c r="D1311" t="str">
+        <v>Swiggy Instamart</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="str">
+        <v>2023-01-11</v>
+      </c>
+      <c r="B1312" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1312">
+        <v>159</v>
+      </c>
+      <c r="D1312" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="str">
+        <v>2023-01-12</v>
+      </c>
+      <c r="B1313" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1313">
+        <v>85</v>
+      </c>
+      <c r="D1313" t="str">
+        <v xml:space="preserve">Swiggy </v>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="str">
+        <v>2023-01-13</v>
+      </c>
+      <c r="B1314" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1314">
+        <v>1277</v>
+      </c>
+      <c r="D1314" t="str">
+        <v>Blinkit</v>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="str">
+        <v>2023-01-17</v>
+      </c>
+      <c r="B1315" t="str">
+        <v>Home</v>
+      </c>
+      <c r="C1315">
+        <v>9000</v>
+      </c>
+      <c r="D1315" t="str">
+        <v>Rent</v>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="str">
+        <v>2023-01-14</v>
+      </c>
+      <c r="B1316" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1316">
+        <v>160</v>
+      </c>
+      <c r="D1316" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="str">
+        <v>2023-01-15</v>
+      </c>
+      <c r="B1317" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1317">
+        <v>152</v>
+      </c>
+      <c r="D1317" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="str">
+        <v>2023-01-15</v>
+      </c>
+      <c r="B1318" t="str">
+        <v>Grocery</v>
+      </c>
+      <c r="C1318">
+        <v>442</v>
+      </c>
+      <c r="D1318" t="str">
+        <v>Bigbasket</v>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="str">
+        <v>2023-01-15</v>
+      </c>
+      <c r="B1319" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1319">
+        <v>100</v>
+      </c>
+      <c r="D1319" t="str">
+        <v>Water</v>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="str">
+        <v>2023-01-15</v>
+      </c>
+      <c r="B1320" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1320">
+        <v>122</v>
+      </c>
+      <c r="D1320" t="str">
+        <v xml:space="preserve">Swiggy </v>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="str">
+        <v>2023-01-17</v>
+      </c>
+      <c r="B1321" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C1321">
+        <v>1000</v>
+      </c>
+      <c r="D1321" t="str">
+        <v>Apple iCloud subscription</v>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="str">
+        <v>2023-01-17</v>
+      </c>
+      <c r="B1322" t="str">
+        <v>Shopping</v>
+      </c>
+      <c r="C1322">
+        <v>7470</v>
+      </c>
+      <c r="D1322" t="str">
+        <v>Abineesha’s Stethoscope</v>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="str">
+        <v>2023-01-17</v>
+      </c>
+      <c r="B1323" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1323">
+        <v>85</v>
+      </c>
+      <c r="D1323" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="str">
+        <v>2023-01-17</v>
+      </c>
+      <c r="B1324" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1324">
+        <v>119</v>
+      </c>
+      <c r="D1324" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="str">
+        <v>2023-01-18</v>
+      </c>
+      <c r="B1325" t="str">
+        <v>Bills</v>
+      </c>
+      <c r="C1325">
+        <v>155</v>
+      </c>
+      <c r="D1325" t="str">
+        <v>Jio Recharge</v>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="str">
+        <v>2023-01-18</v>
+      </c>
+      <c r="B1326" t="str">
+        <v>Food</v>
+      </c>
+      <c r="C1326">
+        <v>85</v>
+      </c>
+      <c r="D1326" t="str">
+        <v>Swiggy</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D1050"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D1326"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>